<commit_message>
Update with CALICE groups
git-svn-id: svn+ssh://svn.cern.ch/reps/jansvn/trunk/lcDetRnD@497 4525493e-7705-40b1-a816-d608a930855b
</commit_message>
<xml_diff>
--- a/ListOfGroups.xlsx
+++ b/ListOfGroups.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="17560" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TPC" sheetId="1" r:id="rId1"/>
     <sheet name="Vertex Detector" sheetId="2" r:id="rId2"/>
     <sheet name="Forward Calorimetry R&amp;D" sheetId="3" r:id="rId3"/>
     <sheet name="US Groups" sheetId="4" r:id="rId4"/>
+    <sheet name="Calice" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="209">
   <si>
     <t>Leader</t>
   </si>
@@ -526,6 +527,167 @@
   </si>
   <si>
     <t>Tim Barklow</t>
+  </si>
+  <si>
+    <t>Si ECAL</t>
+  </si>
+  <si>
+    <t>Vladislav Balagura</t>
+  </si>
+  <si>
+    <t>balagura@llr.in2p3.fr</t>
+  </si>
+  <si>
+    <t>LLR</t>
+  </si>
+  <si>
+    <t>Tamaki Yoshioka</t>
+  </si>
+  <si>
+    <t>yoshioka@phys.kyushu-u.ac.jp</t>
+  </si>
+  <si>
+    <t>Kyushu</t>
+  </si>
+  <si>
+    <t>Sci ECAL</t>
+  </si>
+  <si>
+    <t>Shinshu</t>
+  </si>
+  <si>
+    <r>
+      <t>Tohru Takeshita</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>tohru@shinshu-u.ac.jp</t>
+  </si>
+  <si>
+    <t>MAPS ECAL</t>
+  </si>
+  <si>
+    <t>IC London</t>
+  </si>
+  <si>
+    <t>Paul Dauncey</t>
+  </si>
+  <si>
+    <t>p.dauncey@imperial.ac.uk</t>
+  </si>
+  <si>
+    <t>Sci HCAL</t>
+  </si>
+  <si>
+    <t>Felix Sefkow</t>
+  </si>
+  <si>
+    <t>felix.sefkow@desy.de</t>
+  </si>
+  <si>
+    <t>RPC SDHCAL</t>
+  </si>
+  <si>
+    <t>Lyon</t>
+  </si>
+  <si>
+    <t>laktineh@ipnl.in2p3.fr</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Imad </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Laktineh</t>
+    </r>
+  </si>
+  <si>
+    <t>GEM DHCAL</t>
+  </si>
+  <si>
+    <t>Micromegas SDHCAL</t>
+  </si>
+  <si>
+    <t>Annecy</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Maximilien </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Chefdeville</t>
+    </r>
+  </si>
+  <si>
+    <t>chefdevi@lapp.in2p3.fr</t>
+  </si>
+  <si>
+    <t>Tungsten HCAL</t>
+  </si>
+  <si>
+    <t>Wolfgang Klempt</t>
+  </si>
+  <si>
+    <t>wolfgang.klempt@cern.ch</t>
+  </si>
+  <si>
+    <t>Tail Catcher</t>
+  </si>
+  <si>
+    <t>Vishnu Zutshi</t>
+  </si>
+  <si>
+    <t>NIU / NICADD</t>
+  </si>
+  <si>
+    <t>zutshi@fnal.gov</t>
+  </si>
+  <si>
+    <t>Kiyotomo Kawagoe</t>
+  </si>
+  <si>
+    <t>kawagoe@phys.kyushu-u.ac.jp</t>
+  </si>
+  <si>
+    <t>Jean-Claude Brient</t>
+  </si>
+  <si>
+    <t>brient@llr.in2p3.fr</t>
+  </si>
+  <si>
+    <t>Roman Poeschl</t>
+  </si>
+  <si>
+    <t>LAL: Technical Board</t>
+  </si>
+  <si>
+    <t>poeschl@lal.in2p3.fr</t>
   </si>
 </sst>
 </file>
@@ -533,9 +695,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -567,6 +729,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Courier"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Courier"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -585,14 +774,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -602,69 +792,95 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1005,7 +1221,7 @@
   <cols>
     <col min="1" max="1" width="45.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5" style="2" bestFit="1" customWidth="1"/>
@@ -1014,115 +1230,115 @@
     <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="19" customFormat="1">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:8" s="15" customFormat="1">
+      <c r="A1" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="15" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="20" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="5"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="8"/>
+      <c r="C3" s="20"/>
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="5"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
       <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="10" t="s">
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30">
-      <c r="A8" s="5"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D8" t="s">
@@ -1133,10 +1349,10 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D9" t="s">
@@ -1147,8 +1363,8 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="5"/>
-      <c r="C10" s="8" t="s">
+      <c r="A10" s="19"/>
+      <c r="C10" s="20" t="s">
         <v>30</v>
       </c>
       <c r="D10" t="s">
@@ -1159,8 +1375,8 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="5"/>
-      <c r="C11" s="8"/>
+      <c r="A11" s="19"/>
+      <c r="C11" s="20"/>
       <c r="D11" t="s">
         <v>35</v>
       </c>
@@ -1169,8 +1385,8 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="5"/>
-      <c r="C12" s="9" t="s">
+      <c r="A12" s="19"/>
+      <c r="C12" s="6" t="s">
         <v>37</v>
       </c>
       <c r="D12" t="s">
@@ -1181,10 +1397,10 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D13" t="s">
@@ -1195,8 +1411,8 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="5"/>
-      <c r="C14" s="9" t="s">
+      <c r="A14" s="19"/>
+      <c r="C14" s="6" t="s">
         <v>41</v>
       </c>
       <c r="D14" t="s">
@@ -1207,8 +1423,8 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="5"/>
-      <c r="C15" s="9" t="s">
+      <c r="A15" s="19"/>
+      <c r="C15" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D15" t="s">
@@ -1219,7 +1435,7 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="19" t="s">
         <v>44</v>
       </c>
       <c r="C16" t="s">
@@ -1233,8 +1449,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="30">
-      <c r="A17" s="5"/>
-      <c r="C17" s="6" t="s">
+      <c r="A17" s="19"/>
+      <c r="C17" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D17" t="s">
@@ -1248,12 +1464,12 @@
       <c r="A18" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="6"/>
+      <c r="C18" s="4"/>
       <c r="D18"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="19" t="s">
         <v>51</v>
       </c>
       <c r="C19" t="s">
@@ -1267,7 +1483,7 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="5"/>
+      <c r="A20" s="19"/>
       <c r="C20" t="s">
         <v>45</v>
       </c>
@@ -1279,7 +1495,7 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="19" t="s">
         <v>58</v>
       </c>
       <c r="C21" t="s">
@@ -1293,7 +1509,7 @@
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="5"/>
+      <c r="A22" s="19"/>
       <c r="B22" t="s">
         <v>65</v>
       </c>
@@ -1309,17 +1525,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A5:A8"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A19:A20"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A5:A8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
@@ -1357,136 +1573,136 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5" style="12" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="12"/>
+    <col min="1" max="1" width="39.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" style="9" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="19" customFormat="1">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:8" s="15" customFormat="1">
+      <c r="A1" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="19" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="18"/>
+      <c r="H1" s="21"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="10">
         <v>41690</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="15">
+      <c r="G2" s="12">
         <v>41691</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="9" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="10">
         <v>41694</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="9" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="10">
         <v>41694</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="9" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="10">
         <v>41700</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="9" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="23"/>
-      <c r="B6" s="12" t="s">
+      <c r="A6" s="22"/>
+      <c r="B6" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="9" t="s">
         <v>96</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1494,42 +1710,42 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="10">
         <v>41700</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="9" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="10">
         <v>41708</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="9" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1574,57 +1790,57 @@
     <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="19" customFormat="1">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:8" s="15" customFormat="1">
+      <c r="A1" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="19" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="18"/>
+      <c r="H1" s="21"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="17">
         <v>41690</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="23" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="21">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="17">
         <v>41705</v>
       </c>
-      <c r="F3" s="4"/>
+      <c r="F3" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1652,8 +1868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1666,14 +1882,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
@@ -1757,11 +1973,11 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="19" t="s">
         <v>122</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="19" t="s">
         <v>124</v>
       </c>
       <c r="D8" t="s">
@@ -1772,9 +1988,9 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="5"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="5"/>
+      <c r="C9" s="19"/>
       <c r="D9" t="s">
         <v>126</v>
       </c>
@@ -1797,7 +2013,7 @@
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="23" t="s">
         <v>132</v>
       </c>
       <c r="C11" t="s">
@@ -1811,7 +2027,7 @@
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="4"/>
+      <c r="A12" s="23"/>
       <c r="C12" t="s">
         <v>136</v>
       </c>
@@ -1823,7 +2039,7 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="4"/>
+      <c r="A13" s="23"/>
       <c r="B13" t="s">
         <v>142</v>
       </c>
@@ -1852,7 +2068,7 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="23" t="s">
         <v>147</v>
       </c>
       <c r="C15" t="s">
@@ -1866,7 +2082,7 @@
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="4"/>
+      <c r="A16" s="23"/>
       <c r="C16" t="s">
         <v>150</v>
       </c>
@@ -1906,31 +2122,31 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="B20" s="4"/>
+      <c r="B20" s="23"/>
       <c r="D20" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="23"/>
       <c r="D21" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="23"/>
       <c r="D22" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="23"/>
       <c r="D23" t="s">
         <v>167</v>
       </c>
@@ -1978,4 +2194,260 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="28"/>
+      <c r="D1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="28"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="36">
+      <c r="A4" s="30"/>
+      <c r="B4" s="33" t="s">
+        <v>207</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>206</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="30"/>
+      <c r="B5" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>202</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="30"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="29" t="s">
+        <v>172</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="B8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>184</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" t="s">
+        <v>133</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="29" t="s">
+        <v>186</v>
+      </c>
+      <c r="B11" t="s">
+        <v>187</v>
+      </c>
+      <c r="C11" t="s">
+        <v>189</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="B12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="B13" t="s">
+        <v>192</v>
+      </c>
+      <c r="C13" t="s">
+        <v>193</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="B14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" t="s">
+        <v>196</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="B15" t="s">
+        <v>200</v>
+      </c>
+      <c r="C15" t="s">
+        <v>199</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B2:B3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D6" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="D7" r:id="rId3"/>
+    <hyperlink ref="D8" r:id="rId4"/>
+    <hyperlink ref="D9" r:id="rId5"/>
+    <hyperlink ref="D10" r:id="rId6"/>
+    <hyperlink ref="D11" r:id="rId7"/>
+    <hyperlink ref="D12" r:id="rId8"/>
+    <hyperlink ref="D13" r:id="rId9"/>
+    <hyperlink ref="D14" r:id="rId10"/>
+    <hyperlink ref="D15" r:id="rId11"/>
+    <hyperlink ref="D5" r:id="rId12"/>
+    <hyperlink ref="D3" r:id="rId13"/>
+    <hyperlink ref="D4" r:id="rId14"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updates to the contact list Added an outline .tex document
git-svn-id: svn+ssh://svn.cern.ch/reps/jansvn/trunk/lcDetRnD@502 4525493e-7705-40b1-a816-d608a930855b
</commit_message>
<xml_diff>
--- a/ListOfGroups.xlsx
+++ b/ListOfGroups.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="17560" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="17560" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TPC" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,9 @@
     <sheet name="Calice" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
+  <customWorkbookViews>
+    <customWorkbookView name="Jan Strube - Personal View" guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" mergeInterval="0" personalView="1" yWindow="54" windowWidth="1436" windowHeight="824" tabRatio="500" activeSheetId="4"/>
+  </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -23,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="212">
   <si>
     <t>Leader</t>
   </si>
@@ -688,6 +691,15 @@
   </si>
   <si>
     <t>poeschl@lal.in2p3.fr</t>
+  </si>
+  <si>
+    <t>contacted on</t>
+  </si>
+  <si>
+    <t>response received</t>
+  </si>
+  <si>
+    <t>KPiX_RD_Status.docx</t>
   </si>
 </sst>
 </file>
@@ -782,7 +794,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -832,24 +844,6 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -859,14 +853,8 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -875,6 +863,32 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -887,6 +901,160 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{8C629D3D-FF3D-5D44-8037-C1BB23779435}" diskRevisions="1" revisionId="11" version="2">
+  <header guid="{90EFB229-A129-4641-96FB-C4C9036C70D7}" dateTime="2014-03-18T10:37:43" maxSheetId="6" userName="Jan Strube" r:id="rId1">
+    <sheetIdMap count="5">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{8C629D3D-FF3D-5D44-8037-C1BB23779435}" dateTime="2014-03-18T22:19:39" maxSheetId="6" userName="Jan Strube" r:id="rId2" minRId="1" maxRId="11">
+    <sheetIdMap count="5">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+    </sheetIdMap>
+  </header>
+</headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1" sId="4">
+    <nc r="G1" t="inlineStr">
+      <is>
+        <t>by</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="2" sId="4" odxf="1" dxf="1">
+    <nc r="F1" t="inlineStr">
+      <is>
+        <t>contacted on</t>
+      </is>
+    </nc>
+    <ndxf>
+      <font>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </ndxf>
+  </rcc>
+  <rfmt sheetId="4" sqref="G1" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="3" sId="4">
+    <nc r="G3" t="inlineStr">
+      <is>
+        <t>Jan</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="4" sId="4" odxf="1" dxf="1" numFmtId="21">
+    <nc r="F3">
+      <v>41711</v>
+    </nc>
+    <odxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </odxf>
+    <ndxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="5" sId="4" odxf="1" dxf="1" numFmtId="21">
+    <nc r="F7">
+      <v>41711</v>
+    </nc>
+    <odxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </odxf>
+    <ndxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="6" sId="4">
+    <nc r="G7" t="inlineStr">
+      <is>
+        <t>Jan</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="7" sId="4" odxf="1" dxf="1" numFmtId="21">
+    <nc r="F17">
+      <v>41711</v>
+    </nc>
+    <odxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </odxf>
+    <ndxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="8" sId="4">
+    <nc r="G17" t="inlineStr">
+      <is>
+        <t>Jan</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="9" sId="4">
+    <nc r="H1" t="inlineStr">
+      <is>
+        <t>response received</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="4" sqref="H1" start="0" length="2147483647">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+  </rfmt>
+  <rcc rId="10" sId="4" odxf="1" dxf="1" numFmtId="21">
+    <nc r="H17">
+      <v>41716</v>
+    </nc>
+    <odxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </odxf>
+    <ndxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="11" sId="4">
+    <nc r="I17" t="inlineStr">
+      <is>
+        <t>KPiX_RD_Status.docx</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="delete"/>
+  <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1214,7 +1382,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1237,10 +1405,10 @@
       <c r="B1" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="21"/>
+      <c r="D1" s="28"/>
       <c r="E1" s="15" t="s">
         <v>1</v>
       </c>
@@ -1255,11 +1423,11 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="26" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="27" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1270,9 +1438,9 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="19"/>
+      <c r="A3" s="26"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="20"/>
+      <c r="C3" s="27"/>
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1281,7 +1449,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="19"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="3"/>
       <c r="C4" s="6" t="s">
         <v>7</v>
@@ -1294,10 +1462,10 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="26" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -1311,8 +1479,8 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
       <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
@@ -1321,8 +1489,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="30">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
       <c r="C7" s="7" t="s">
         <v>20</v>
       </c>
@@ -1334,7 +1502,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="30">
-      <c r="A8" s="19"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
@@ -1349,7 +1517,7 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="26" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -1363,8 +1531,8 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="19"/>
-      <c r="C10" s="20" t="s">
+      <c r="A10" s="26"/>
+      <c r="C10" s="27" t="s">
         <v>30</v>
       </c>
       <c r="D10" t="s">
@@ -1375,8 +1543,8 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="19"/>
-      <c r="C11" s="20"/>
+      <c r="A11" s="26"/>
+      <c r="C11" s="27"/>
       <c r="D11" t="s">
         <v>35</v>
       </c>
@@ -1385,7 +1553,7 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="19"/>
+      <c r="A12" s="26"/>
       <c r="C12" s="6" t="s">
         <v>37</v>
       </c>
@@ -1397,7 +1565,7 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="26" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -1411,7 +1579,7 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="19"/>
+      <c r="A14" s="26"/>
       <c r="C14" s="6" t="s">
         <v>41</v>
       </c>
@@ -1423,7 +1591,7 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="19"/>
+      <c r="A15" s="26"/>
       <c r="C15" s="6" t="s">
         <v>29</v>
       </c>
@@ -1435,7 +1603,7 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="26" t="s">
         <v>44</v>
       </c>
       <c r="C16" t="s">
@@ -1449,7 +1617,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="30">
-      <c r="A17" s="19"/>
+      <c r="A17" s="26"/>
       <c r="C17" s="4" t="s">
         <v>48</v>
       </c>
@@ -1469,7 +1637,7 @@
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="26" t="s">
         <v>51</v>
       </c>
       <c r="C19" t="s">
@@ -1483,7 +1651,7 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="19"/>
+      <c r="A20" s="26"/>
       <c r="C20" t="s">
         <v>45</v>
       </c>
@@ -1495,7 +1663,7 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="26" t="s">
         <v>58</v>
       </c>
       <c r="C21" t="s">
@@ -1509,7 +1677,7 @@
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="19"/>
+      <c r="A22" s="26"/>
       <c r="B22" t="s">
         <v>65</v>
       </c>
@@ -1524,6 +1692,12 @@
       </c>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
+      <selection activeCell="E24" sqref="E24"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+  </customSheetViews>
   <mergeCells count="11">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C2:C3"/>
@@ -1573,8 +1747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1584,19 +1758,19 @@
     <col min="3" max="3" width="16.5" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.33203125" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5" style="9" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="9"/>
+    <col min="6" max="7" width="6.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="15" customFormat="1">
       <c r="A1" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21"/>
+      <c r="C1" s="28"/>
       <c r="D1" s="15" t="s">
         <v>1</v>
       </c>
@@ -1606,10 +1780,10 @@
       <c r="F1" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="21"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="8" t="s">
@@ -1678,7 +1852,7 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="29" t="s">
         <v>82</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -1698,7 +1872,7 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="22"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="9" t="s">
         <v>52</v>
       </c>
@@ -1750,6 +1924,12 @@
       </c>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
+      <selection activeCell="A4" sqref="A4"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+  </customSheetViews>
   <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="G1:H1"/>
@@ -1794,10 +1974,10 @@
       <c r="A1" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21"/>
+      <c r="C1" s="28"/>
       <c r="D1" s="15" t="s">
         <v>1</v>
       </c>
@@ -1807,42 +1987,47 @@
       <c r="F1" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="21"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="31" t="s">
         <v>95</v>
       </c>
       <c r="E2" s="17">
         <v>41690</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="30" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="24"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="31"/>
       <c r="E3" s="17">
         <v>41705</v>
       </c>
-      <c r="F3" s="23"/>
+      <c r="F3" s="30"/>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
+      <selection activeCell="F2" sqref="F2:F3"/>
+    </customSheetView>
+  </customSheetViews>
   <mergeCells count="7">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="G1:H1"/>
@@ -1866,10 +2051,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1879,9 +2064,10 @@
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" s="18" t="s">
         <v>98</v>
       </c>
@@ -1889,9 +2075,17 @@
       <c r="C1" s="18"/>
       <c r="D1" s="18"/>
       <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="F1" s="34" t="s">
+        <v>209</v>
+      </c>
+      <c r="G1" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="35" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -1905,7 +2099,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>103</v>
       </c>
@@ -1918,8 +2112,14 @@
       <c r="E3" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="F3" s="17">
+        <v>41711</v>
+      </c>
+      <c r="G3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>107</v>
       </c>
@@ -1933,7 +2133,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>111</v>
       </c>
@@ -1947,7 +2147,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>115</v>
       </c>
@@ -1961,7 +2161,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:8">
       <c r="C7" t="s">
         <v>87</v>
       </c>
@@ -1971,13 +2171,19 @@
       <c r="E7" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="19" t="s">
+      <c r="F7" s="17">
+        <v>41711</v>
+      </c>
+      <c r="G7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="26" t="s">
         <v>122</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="26" t="s">
         <v>124</v>
       </c>
       <c r="D8" t="s">
@@ -1987,10 +2193,10 @@
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="19"/>
+    <row r="9" spans="1:8">
+      <c r="A9" s="26"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="19"/>
+      <c r="C9" s="26"/>
       <c r="D9" t="s">
         <v>126</v>
       </c>
@@ -1998,7 +2204,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>128</v>
       </c>
@@ -2012,8 +2218,8 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="23" t="s">
+    <row r="11" spans="1:8">
+      <c r="A11" s="30" t="s">
         <v>132</v>
       </c>
       <c r="C11" t="s">
@@ -2026,8 +2232,8 @@
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="23"/>
+    <row r="12" spans="1:8">
+      <c r="A12" s="30"/>
       <c r="C12" t="s">
         <v>136</v>
       </c>
@@ -2038,8 +2244,8 @@
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="23"/>
+    <row r="13" spans="1:8">
+      <c r="A13" s="30"/>
       <c r="B13" t="s">
         <v>142</v>
       </c>
@@ -2053,7 +2259,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>143</v>
       </c>
@@ -2067,8 +2273,8 @@
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="23" t="s">
+    <row r="15" spans="1:8">
+      <c r="A15" s="30" t="s">
         <v>147</v>
       </c>
       <c r="C15" t="s">
@@ -2081,8 +2287,8 @@
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="23"/>
+    <row r="16" spans="1:8">
+      <c r="A16" s="30"/>
       <c r="C16" t="s">
         <v>150</v>
       </c>
@@ -2093,7 +2299,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>153</v>
       </c>
@@ -2106,8 +2312,20 @@
       <c r="E17" s="1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" s="17">
+        <v>41711</v>
+      </c>
+      <c r="G17" t="s">
+        <v>78</v>
+      </c>
+      <c r="H17" s="17">
+        <v>41716</v>
+      </c>
+      <c r="I17" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>157</v>
       </c>
@@ -2121,37 +2339,37 @@
         <v>159</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="23" t="s">
+    <row r="20" spans="1:9">
+      <c r="A20" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="B20" s="23"/>
+      <c r="B20" s="30"/>
       <c r="D20" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="23"/>
-      <c r="B21" s="23"/>
+    <row r="21" spans="1:9">
+      <c r="A21" s="30"/>
+      <c r="B21" s="30"/>
       <c r="D21" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="23"/>
-      <c r="B22" s="23"/>
+    <row r="22" spans="1:9">
+      <c r="A22" s="30"/>
+      <c r="B22" s="30"/>
       <c r="D22" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="23"/>
-      <c r="B23" s="23"/>
+    <row r="23" spans="1:9">
+      <c r="A23" s="30"/>
+      <c r="B23" s="30"/>
       <c r="D23" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>162</v>
       </c>
@@ -2160,6 +2378,12 @@
       </c>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
+      <selection activeCell="H17" sqref="H17"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+  </customSheetViews>
   <mergeCells count="5">
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="C8:C9"/>
@@ -2200,8 +2424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2214,35 +2438,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="26" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="28"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="33" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="33" t="s">
         <v>171</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="22" t="s">
         <v>169</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -2250,9 +2474,9 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="32" t="s">
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="24" t="s">
         <v>204</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -2260,11 +2484,11 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="36">
-      <c r="A4" s="30"/>
-      <c r="B4" s="33" t="s">
+      <c r="A4" s="33"/>
+      <c r="B4" s="25" t="s">
         <v>207</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="24" t="s">
         <v>206</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -2272,11 +2496,11 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="30"/>
-      <c r="B5" s="23" t="s">
+      <c r="A5" s="33"/>
+      <c r="B5" s="30" t="s">
         <v>174</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="24" t="s">
         <v>202</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -2284,9 +2508,9 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="30"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="29" t="s">
+      <c r="A6" s="33"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="22" t="s">
         <v>172</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -2294,13 +2518,13 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="23" t="s">
         <v>177</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -2308,7 +2532,7 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="22" t="s">
         <v>179</v>
       </c>
       <c r="B8" t="s">
@@ -2322,7 +2546,7 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="22" t="s">
         <v>183</v>
       </c>
       <c r="B9" t="s">
@@ -2336,7 +2560,7 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="22" t="s">
         <v>132</v>
       </c>
       <c r="B10" t="s">
@@ -2350,7 +2574,7 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="22" t="s">
         <v>186</v>
       </c>
       <c r="B11" t="s">
@@ -2364,7 +2588,7 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="22" t="s">
         <v>190</v>
       </c>
       <c r="B12" t="s">
@@ -2378,7 +2602,7 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="22" t="s">
         <v>191</v>
       </c>
       <c r="B13" t="s">
@@ -2392,7 +2616,7 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="22" t="s">
         <v>195</v>
       </c>
       <c r="B14" t="s">
@@ -2406,7 +2630,7 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="22" t="s">
         <v>198</v>
       </c>
       <c r="B15" t="s">
@@ -2420,6 +2644,11 @@
       </c>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
+      <selection activeCell="B8" sqref="B8"/>
+    </customSheetView>
+  </customSheetViews>
   <mergeCells count="5">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="G1:H1"/>

</xml_diff>

<commit_message>
Updates to the list of contacted groups
git-svn-id: svn+ssh://svn.cern.ch/reps/jansvn/trunk/lcDetRnD@508 4525493e-7705-40b1-a816-d608a930855b
</commit_message>
<xml_diff>
--- a/ListOfGroups.xlsx
+++ b/ListOfGroups.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="0" windowWidth="28720" windowHeight="17380" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-40" yWindow="0" windowWidth="28720" windowHeight="17380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TPC" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,8 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="TITOV Maksym - Personal View" guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1243" windowHeight="652" tabRatio="500" activeSheetId="2"/>
     <customWorkbookView name="Jan Strube - Personal View" guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" mergeInterval="0" personalView="1" xWindow="-2" yWindow="54" windowWidth="1436" windowHeight="815" tabRatio="500" activeSheetId="2"/>
-    <customWorkbookView name="TITOV Maksym - Personal View" guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1243" windowHeight="652" tabRatio="500" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="227">
   <si>
     <t>Leader</t>
   </si>
@@ -562,6 +562,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -743,6 +744,12 @@
   <si>
     <t>ruiz@ifca.unican.es</t>
   </si>
+  <si>
+    <t>Dominik Dannheim</t>
+  </si>
+  <si>
+    <t>dominik.dannheim@cern.ch</t>
+  </si>
 </sst>
 </file>
 
@@ -757,6 +764,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -836,7 +844,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -915,14 +923,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -939,10 +954,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -963,7 +974,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{AD5617E4-C62E-0746-A7C9-5D96D7D4DE27}" diskRevisions="1" revisionId="92" version="2">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{DB2702CC-435E-D146-B4C9-AE60ADA8C4EB}" diskRevisions="1" revisionId="106" version="3">
   <header guid="{90EFB229-A129-4641-96FB-C4C9036C70D7}" dateTime="2014-03-18T10:37:43" maxSheetId="6" userName="Jan Strube" r:id="rId1">
     <sheetIdMap count="5">
       <sheetId val="1"/>
@@ -1164,6 +1175,17 @@
       <sheetId val="7"/>
     </sheetIdMap>
   </header>
+  <header guid="{DB2702CC-435E-D146-B4C9-AE60ADA8C4EB}" dateTime="2014-03-25T17:00:47" maxSheetId="8" userName="Jan Strube" r:id="rId22" minRId="93" maxRId="106">
+    <sheetIdMap count="7">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -1966,6 +1988,97 @@
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="delete"/>
   <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog22.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="93" sId="2">
+    <nc r="A14" t="inlineStr">
+      <is>
+        <t>CLIC</t>
+      </is>
+    </nc>
+  </rcc>
+  <rrc rId="94" sId="2" ref="A15:XFD15" action="insertRow"/>
+  <rcc rId="95" sId="2">
+    <nc r="C15" t="inlineStr">
+      <is>
+        <t>Dominik Dannheim</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="96" sId="2">
+    <nc r="D15" t="inlineStr">
+      <is>
+        <t>dominik.dannheim@cern.ch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="97" sId="2" numFmtId="19">
+    <nc r="E15">
+      <v>41723</v>
+    </nc>
+  </rcc>
+  <rcc rId="98" sId="2">
+    <nc r="F15" t="inlineStr">
+      <is>
+        <t>Jan</t>
+      </is>
+    </nc>
+  </rcc>
+  <rrc rId="99" sId="2" ref="A9:XFD9" action="insertRow"/>
+  <rcc rId="100" sId="2" numFmtId="19">
+    <nc r="E9">
+      <v>41723</v>
+    </nc>
+  </rcc>
+  <rrc rId="101" sId="5" ref="A13:XFD13" action="insertRow"/>
+  <rcc rId="102" sId="5" numFmtId="19">
+    <nc r="E13">
+      <v>41723</v>
+    </nc>
+  </rcc>
+  <rcc rId="103" sId="5" odxf="1" dxf="1" numFmtId="21">
+    <nc r="G7">
+      <v>41723</v>
+    </nc>
+    <odxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </odxf>
+    <ndxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="104" sId="5" odxf="1" dxf="1" numFmtId="21">
+    <nc r="E18">
+      <v>41723</v>
+    </nc>
+    <odxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </odxf>
+    <ndxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="105" sId="1" odxf="1" dxf="1" numFmtId="21">
+    <nc r="F4">
+      <v>41715</v>
+    </nc>
+    <odxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </odxf>
+    <ndxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="106" sId="1">
+    <nc r="G4" t="inlineStr">
+      <is>
+        <t>Jan</t>
+      </is>
+    </nc>
+  </rcc>
 </revisions>
 </file>
 
@@ -2718,8 +2831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2742,10 +2855,10 @@
       <c r="B1" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="32"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="15" t="s">
         <v>1</v>
       </c>
@@ -2760,11 +2873,11 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="35" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="36" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -2775,9 +2888,9 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="34"/>
+      <c r="A3" s="35"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="33"/>
+      <c r="C3" s="36"/>
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
@@ -2786,7 +2899,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="34"/>
+      <c r="A4" s="35"/>
       <c r="B4" s="3"/>
       <c r="C4" s="6" t="s">
         <v>7</v>
@@ -2797,12 +2910,18 @@
       <c r="E4" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="F4" s="33">
+        <v>41715</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -2816,8 +2935,8 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="35"/>
       <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
@@ -2825,9 +2944,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="31.5">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
+    <row r="7" spans="1:8" ht="30">
+      <c r="A7" s="35"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="7" t="s">
         <v>20</v>
       </c>
@@ -2838,8 +2957,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="31.5">
-      <c r="A8" s="34"/>
+    <row r="8" spans="1:8" ht="30">
+      <c r="A8" s="35"/>
       <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
@@ -2854,7 +2973,7 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="35" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -2868,8 +2987,8 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="34"/>
-      <c r="C10" s="33" t="s">
+      <c r="A10" s="35"/>
+      <c r="C10" s="36" t="s">
         <v>30</v>
       </c>
       <c r="D10" t="s">
@@ -2880,8 +2999,8 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="34"/>
-      <c r="C11" s="33"/>
+      <c r="A11" s="35"/>
+      <c r="C11" s="36"/>
       <c r="D11" t="s">
         <v>35</v>
       </c>
@@ -2890,7 +3009,7 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="34"/>
+      <c r="A12" s="35"/>
       <c r="C12" s="6" t="s">
         <v>37</v>
       </c>
@@ -2902,7 +3021,7 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="35" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -2916,7 +3035,7 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="34"/>
+      <c r="A14" s="35"/>
       <c r="C14" s="6" t="s">
         <v>41</v>
       </c>
@@ -2928,7 +3047,7 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="34"/>
+      <c r="A15" s="35"/>
       <c r="C15" s="6" t="s">
         <v>29</v>
       </c>
@@ -2940,7 +3059,7 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="35" t="s">
         <v>44</v>
       </c>
       <c r="C16" t="s">
@@ -2953,8 +3072,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="31.5">
-      <c r="A17" s="34"/>
+    <row r="17" spans="1:9" ht="30">
+      <c r="A17" s="35"/>
       <c r="C17" s="4" t="s">
         <v>48</v>
       </c>
@@ -2974,7 +3093,7 @@
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="35" t="s">
         <v>51</v>
       </c>
       <c r="C19" t="s">
@@ -2988,7 +3107,7 @@
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="34"/>
+      <c r="A20" s="35"/>
       <c r="C20" t="s">
         <v>45</v>
       </c>
@@ -3000,7 +3119,7 @@
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="35" t="s">
         <v>58</v>
       </c>
       <c r="C21" t="s">
@@ -3014,7 +3133,7 @@
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="34"/>
+      <c r="A22" s="35"/>
       <c r="B22" t="s">
         <v>65</v>
       </c>
@@ -3040,7 +3159,7 @@
       <c r="E24" s="30" t="s">
         <v>215</v>
       </c>
-      <c r="F24" s="40">
+      <c r="F24" s="33">
         <v>41710</v>
       </c>
       <c r="G24" s="29" t="s">
@@ -3055,27 +3174,27 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
+      <selection activeCell="E24" sqref="E24"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" topLeftCell="B1">
       <selection activeCell="H24" sqref="H24"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
-      <selection activeCell="E24" sqref="E24"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
   </customSheetViews>
   <mergeCells count="11">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A5:A8"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A19:A20"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A5:A8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
@@ -3099,7 +3218,7 @@
     <hyperlink ref="E21" r:id="rId19"/>
     <hyperlink ref="E22" r:id="rId20"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -3111,10 +3230,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E8:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3134,10 +3253,10 @@
       <c r="A1" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="32"/>
+      <c r="C1" s="37"/>
       <c r="D1" s="15" t="s">
         <v>1</v>
       </c>
@@ -3147,10 +3266,10 @@
       <c r="F1" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="32"/>
+      <c r="H1" s="37"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="8" t="s">
@@ -3219,7 +3338,7 @@
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="38" t="s">
         <v>82</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -3239,7 +3358,7 @@
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="35"/>
+      <c r="A6" s="38"/>
       <c r="B6" s="9" t="s">
         <v>52</v>
       </c>
@@ -3291,99 +3410,122 @@
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" t="s">
+      <c r="D9" s="32"/>
+      <c r="E9" s="10">
+        <v>41723</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
         <v>150</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B10" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>152</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>153</v>
       </c>
-      <c r="E9" s="31">
+      <c r="E10" s="31">
         <v>41711</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F10" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G10" s="28">
         <v>41716</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="H10" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I10" t="s">
         <v>208</v>
       </c>
-      <c r="J9"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="B11" s="9" t="s">
+      <c r="J10"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="B12" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C12" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>105</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E12" s="28">
         <v>41711</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="B14" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="E14" s="10">
-        <v>41718</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>72</v>
-      </c>
+      <c r="G12" s="17"/>
+      <c r="H12"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="E15" s="10">
+        <v>41718</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="C16" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="E16" s="10">
+        <v>41723</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B17" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C17" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D17" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E17" s="10">
         <v>41721</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F17" s="9" t="s">
         <v>78</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" topLeftCell="B1">
+      <selection activeCell="F14" sqref="F14"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
       <selection activeCell="F7" sqref="F7"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" topLeftCell="B1">
-      <selection activeCell="F14" sqref="F14"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
@@ -3400,7 +3542,7 @@
     <hyperlink ref="D8" r:id="rId5"/>
     <hyperlink ref="D6" r:id="rId6"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -3431,10 +3573,10 @@
       <c r="A1" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="32"/>
+      <c r="C1" s="37"/>
       <c r="D1" s="15" t="s">
         <v>1</v>
       </c>
@@ -3444,48 +3586,48 @@
       <c r="F1" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="32"/>
+      <c r="H1" s="37"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="40" t="s">
         <v>95</v>
       </c>
       <c r="E2" s="17">
         <v>41690</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="39" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="36"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="37"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="40"/>
       <c r="E3" s="17">
         <v>41718</v>
       </c>
-      <c r="F3" s="36"/>
+      <c r="F3" s="39"/>
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
+      <selection activeCell="E3" sqref="E3"/>
+    </customSheetView>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
       <selection activeCell="F2" sqref="F2:F3"/>
-    </customSheetView>
-    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
-      <selection activeCell="E3" sqref="E3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="7">
@@ -3500,7 +3642,7 @@
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3653,7 +3795,7 @@
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="39" t="s">
         <v>129</v>
       </c>
       <c r="C9" t="s">
@@ -3667,7 +3809,7 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="36"/>
+      <c r="A10" s="39"/>
       <c r="C10" t="s">
         <v>133</v>
       </c>
@@ -3679,7 +3821,7 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="36"/>
+      <c r="A11" s="39"/>
       <c r="B11" t="s">
         <v>139</v>
       </c>
@@ -3708,7 +3850,7 @@
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="39" t="s">
         <v>144</v>
       </c>
       <c r="C13" t="s">
@@ -3722,7 +3864,7 @@
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="36"/>
+      <c r="A14" s="39"/>
       <c r="C14" t="s">
         <v>147</v>
       </c>
@@ -3774,31 +3916,31 @@
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="B18" s="36"/>
+      <c r="B18" s="39"/>
       <c r="D18" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="39"/>
+      <c r="B19" s="39"/>
       <c r="D19" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="36"/>
-      <c r="B20" s="36"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="39"/>
       <c r="D20" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="36"/>
-      <c r="B21" s="36"/>
+      <c r="A21" s="39"/>
+      <c r="B21" s="39"/>
       <c r="D21" t="s">
         <v>164</v>
       </c>
@@ -3813,12 +3955,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
+      <selection activeCell="C7" sqref="C7"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
       <selection activeCell="C16" sqref="C16"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
-      <selection activeCell="C7" sqref="C7"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
@@ -3844,7 +3986,7 @@
     <hyperlink ref="E15" r:id="rId14"/>
     <hyperlink ref="E16" r:id="rId15"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -3856,10 +3998,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3875,10 +4017,10 @@
       <c r="A1" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="38"/>
+      <c r="C1" s="41"/>
       <c r="D1" s="20" t="s">
         <v>1</v>
       </c>
@@ -3888,16 +4030,16 @@
       <c r="F1" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="38"/>
+      <c r="H1" s="41"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="42" t="s">
         <v>165</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="42" t="s">
         <v>168</v>
       </c>
       <c r="C2" s="22" t="s">
@@ -3908,8 +4050,8 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="39"/>
-      <c r="B3" s="39"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="42"/>
       <c r="C3" s="24" t="s">
         <v>201</v>
       </c>
@@ -3924,7 +4066,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="36">
-      <c r="A4" s="39"/>
+      <c r="A4" s="42"/>
       <c r="B4" s="25" t="s">
         <v>204</v>
       </c>
@@ -3942,8 +4084,8 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="39"/>
-      <c r="B5" s="36" t="s">
+      <c r="A5" s="42"/>
+      <c r="B5" s="39" t="s">
         <v>171</v>
       </c>
       <c r="C5" s="24" t="s">
@@ -3960,8 +4102,8 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="39"/>
-      <c r="B6" s="36"/>
+      <c r="A6" s="42"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="22" t="s">
         <v>169</v>
       </c>
@@ -3988,6 +4130,9 @@
       <c r="F7" t="s">
         <v>78</v>
       </c>
+      <c r="G7" s="17">
+        <v>41723</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="22" t="s">
@@ -4090,123 +4235,135 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="22" t="s">
-        <v>188</v>
-      </c>
-      <c r="B13" t="s">
-        <v>189</v>
-      </c>
-      <c r="C13" t="s">
-        <v>190</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>191</v>
-      </c>
+      <c r="A13" s="22"/>
+      <c r="D13" s="1"/>
       <c r="E13" s="28">
-        <v>41717</v>
-      </c>
-      <c r="F13" t="s">
-        <v>72</v>
+        <v>41723</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="22" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>189</v>
       </c>
       <c r="C14" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
+      </c>
+      <c r="E14" s="28">
+        <v>41717</v>
+      </c>
+      <c r="F14" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="22" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B15" t="s">
-        <v>197</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="B16" t="s">
+        <v>197</v>
+      </c>
+      <c r="C16" t="s">
+        <v>196</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>87</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>118</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E16" s="28">
+      <c r="E17" s="28">
         <v>41711</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F17" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="22" t="s">
+      <c r="E18" s="17">
+        <v>41723</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="22" t="s">
         <v>217</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>218</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>219</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>220</v>
       </c>
-      <c r="E18" s="41">
+      <c r="E19" s="34">
         <v>41718</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
-      <c r="A23" t="s">
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
         <v>210</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>151</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>152</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>153</v>
       </c>
-      <c r="E23" s="28">
+      <c r="E24" s="28">
         <v>41711</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F24" t="s">
         <v>78</v>
       </c>
-      <c r="G23" s="28">
+      <c r="G24" s="28">
         <v>41716</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H24" t="s">
         <v>208</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
+      <selection activeCell="F8" sqref="F8"/>
+    </customSheetView>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
       <selection activeCell="D18" sqref="D18"/>
-    </customSheetView>
-    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
-      <selection activeCell="F8" sqref="F8"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="5">
@@ -4225,14 +4382,14 @@
     <hyperlink ref="D10" r:id="rId6"/>
     <hyperlink ref="D11" r:id="rId7"/>
     <hyperlink ref="D12" r:id="rId8"/>
-    <hyperlink ref="D13" r:id="rId9"/>
-    <hyperlink ref="D14" r:id="rId10"/>
-    <hyperlink ref="D15" r:id="rId11"/>
+    <hyperlink ref="D14" r:id="rId9"/>
+    <hyperlink ref="D15" r:id="rId10"/>
+    <hyperlink ref="D16" r:id="rId11"/>
     <hyperlink ref="D5" r:id="rId12"/>
     <hyperlink ref="D3" r:id="rId13"/>
     <hyperlink ref="D4" r:id="rId14"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4250,10 +4407,10 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
   <customSheetViews>
+    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}"/>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}"/>
-    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}"/>
   </customSheetViews>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Additions to the List of groups and the bibliography
git-svn-id: svn+ssh://svn.cern.ch/reps/jansvn/trunk/lcDetRnD@525 4525493e-7705-40b1-a816-d608a930855b
</commit_message>
<xml_diff>
--- a/ListOfGroups.xlsx
+++ b/ListOfGroups.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="0" windowWidth="28720" windowHeight="17380" tabRatio="500"/>
+    <workbookView xWindow="-40" yWindow="0" windowWidth="28720" windowHeight="17380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TPC" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,8 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jan Strube - Personal View" guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" mergeInterval="0" personalView="1" xWindow="-2" yWindow="54" windowWidth="1436" windowHeight="815" tabRatio="500" activeSheetId="2"/>
     <customWorkbookView name="TITOV Maksym - Personal View" guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1243" windowHeight="652" tabRatio="500" activeSheetId="2"/>
-    <customWorkbookView name="Jan Strube - Personal View" guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" mergeInterval="0" personalView="1" xWindow="-2" yWindow="54" windowWidth="1436" windowHeight="815" tabRatio="500" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="230">
   <si>
     <t>Leader</t>
   </si>
@@ -697,9 +697,6 @@
     <t>KPiX_RD_Status.docx</t>
   </si>
   <si>
-    <t>Report received</t>
-  </si>
-  <si>
     <t>KPIX</t>
   </si>
   <si>
@@ -749,6 +746,18 @@
   </si>
   <si>
     <t>dominik.dannheim@cern.ch</t>
+  </si>
+  <si>
+    <t>FPCCD_VTX_YasuhiroSugimoto_KEK_20140403.docx</t>
+  </si>
+  <si>
+    <t>Tracker_KPIX_MartyBreidenbach_SLAC_20140318.docx</t>
+  </si>
+  <si>
+    <t>Chronopixel_NickSinev_Oregon_20140405.docx</t>
+  </si>
+  <si>
+    <t>Tracker_SCIPPTracking_BruceSchumm_SCIPP_20140326.docx</t>
   </si>
 </sst>
 </file>
@@ -836,15 +845,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -866,18 +876,12 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -933,11 +937,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -954,12 +964,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -974,7 +987,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{DB2702CC-435E-D146-B4C9-AE60ADA8C4EB}" diskRevisions="1" revisionId="106" version="3">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{FAE6AD53-8B02-964B-9E03-2DA6A505E01F}" diskRevisions="1" revisionId="113" version="4">
   <header guid="{90EFB229-A129-4641-96FB-C4C9036C70D7}" dateTime="2014-03-18T10:37:43" maxSheetId="6" userName="Jan Strube" r:id="rId1">
     <sheetIdMap count="5">
       <sheetId val="1"/>
@@ -1186,6 +1199,17 @@
       <sheetId val="7"/>
     </sheetIdMap>
   </header>
+  <header guid="{FAE6AD53-8B02-964B-9E03-2DA6A505E01F}" dateTime="2014-04-05T13:14:05" maxSheetId="8" userName="Jan Strube" r:id="rId23" minRId="107" maxRId="113">
+    <sheetIdMap count="7">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -2082,6 +2106,128 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog23.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="107" sId="2" odxf="1" dxf="1" numFmtId="21">
+    <nc r="G4">
+      <v>41732</v>
+    </nc>
+    <odxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </odxf>
+    <ndxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </ndxf>
+  </rcc>
+  <rfmt sheetId="2" xfDxf="1" sqref="H4" start="0" length="0">
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="108" sId="2">
+    <nc r="H4" t="inlineStr">
+      <is>
+        <t>FPCCD_VTX_YasuhiroSugimoto_KEK_20140403.docx</t>
+      </is>
+    </nc>
+  </rcc>
+  <rm rId="109" sheetId="2" source="I10" destination="H10" sourceSheetId="2">
+    <rcc rId="0" sId="2" dxf="1">
+      <nc r="H10" t="inlineStr">
+        <is>
+          <t>Report received</t>
+        </is>
+      </nc>
+      <ndxf>
+        <numFmt numFmtId="21" formatCode="d\-mmm"/>
+      </ndxf>
+    </rcc>
+  </rm>
+  <rcc rId="110" sId="2" xfDxf="1" dxf="1">
+    <oc r="H10" t="inlineStr">
+      <is>
+        <t>KPiX_RD_Status.docx</t>
+      </is>
+    </oc>
+    <nc r="H10" t="inlineStr">
+      <is>
+        <t>Tracker_KPIX_MartyBreidenbach_SLAC_20140318.docx</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="2" sqref="A1:A1048576">
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="2" sqref="A1:A1048576">
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="2" sqref="A1:A1048576">
+    <dxf>
+      <alignment horizontal="general"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="2" sqref="A1:A1048576">
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="2" sqref="A1:A1048576">
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="111" sId="2" odxf="1" dxf="1" numFmtId="21">
+    <nc r="G7">
+      <v>41734</v>
+    </nc>
+    <odxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </odxf>
+    <ndxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="112" sId="2" xfDxf="1" dxf="1">
+    <nc r="H7" t="inlineStr">
+      <is>
+        <t>Chronopixel_NickSinev_Oregon_20140405.docx</t>
+      </is>
+    </nc>
+    <ndxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="113" sId="2" xfDxf="1" dxf="1">
+    <nc r="H12" t="inlineStr">
+      <is>
+        <t>Tracker_SCIPPTracking_BruceSchumm_SCIPP_20140326.docx</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="2" sqref="G1:G1048576">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="2" sqref="G1:G1048576">
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="2" sqref="G1:G1048576">
+    <dxf>
+      <alignment horizontal="general"/>
+    </dxf>
+  </rfmt>
+  <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="delete"/>
+  <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="12" sId="5" odxf="1" dxf="1" numFmtId="19">
@@ -2504,7 +2650,9 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+  <userInfo guid="{FAE6AD53-8B02-964B-9E03-2DA6A505E01F}" name="Jan Strube" id="-985427944" dateTime="2014-04-05T13:05:11"/>
+</users>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2831,8 +2979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2848,32 +2996,32 @@
     <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="15" customFormat="1">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:8" s="13" customFormat="1">
+      <c r="A1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="15" t="s">
+      <c r="D1" s="35"/>
+      <c r="E1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="37" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3"/>
@@ -2888,7 +3036,7 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="35"/>
+      <c r="A3" s="37"/>
       <c r="B3" s="3"/>
       <c r="C3" s="36"/>
       <c r="D3" s="2" t="s">
@@ -2899,7 +3047,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="35"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="3"/>
       <c r="C4" s="6" t="s">
         <v>7</v>
@@ -2910,7 +3058,7 @@
       <c r="E4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="33">
+      <c r="F4" s="31">
         <v>41715</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -2918,10 +3066,10 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="37" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -2935,8 +3083,8 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="35"/>
-      <c r="B6" s="35"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="37"/>
       <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
@@ -2945,8 +3093,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="30">
-      <c r="A7" s="35"/>
-      <c r="B7" s="35"/>
+      <c r="A7" s="37"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="7" t="s">
         <v>20</v>
       </c>
@@ -2958,7 +3106,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="30">
-      <c r="A8" s="35"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
@@ -2973,7 +3121,7 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="37" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -2987,7 +3135,7 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="35"/>
+      <c r="A10" s="37"/>
       <c r="C10" s="36" t="s">
         <v>30</v>
       </c>
@@ -2999,7 +3147,7 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="35"/>
+      <c r="A11" s="37"/>
       <c r="C11" s="36"/>
       <c r="D11" t="s">
         <v>35</v>
@@ -3009,7 +3157,7 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="35"/>
+      <c r="A12" s="37"/>
       <c r="C12" s="6" t="s">
         <v>37</v>
       </c>
@@ -3021,7 +3169,7 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="37" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -3035,7 +3183,7 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="35"/>
+      <c r="A14" s="37"/>
       <c r="C14" s="6" t="s">
         <v>41</v>
       </c>
@@ -3047,7 +3195,7 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="35"/>
+      <c r="A15" s="37"/>
       <c r="C15" s="6" t="s">
         <v>29</v>
       </c>
@@ -3059,7 +3207,7 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="37" t="s">
         <v>44</v>
       </c>
       <c r="C16" t="s">
@@ -3073,7 +3221,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="30">
-      <c r="A17" s="35"/>
+      <c r="A17" s="37"/>
       <c r="C17" s="4" t="s">
         <v>48</v>
       </c>
@@ -3093,7 +3241,7 @@
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="37" t="s">
         <v>51</v>
       </c>
       <c r="C19" t="s">
@@ -3107,7 +3255,7 @@
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="35"/>
+      <c r="A20" s="37"/>
       <c r="C20" t="s">
         <v>45</v>
       </c>
@@ -3119,7 +3267,7 @@
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="37" t="s">
         <v>58</v>
       </c>
       <c r="C21" t="s">
@@ -3133,7 +3281,7 @@
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="35"/>
+      <c r="A22" s="37"/>
       <c r="B22" t="s">
         <v>65</v>
       </c>
@@ -3148,53 +3296,53 @@
       </c>
     </row>
     <row r="24" spans="1:9" customFormat="1">
-      <c r="A24" s="27"/>
+      <c r="A24" s="25"/>
       <c r="B24" s="2"/>
       <c r="C24" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="29" t="s">
+      <c r="D24" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="E24" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="E24" s="30" t="s">
+      <c r="F24" s="31">
+        <v>41710</v>
+      </c>
+      <c r="G24" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="H24" s="15">
+        <v>41712</v>
+      </c>
+      <c r="I24" t="s">
         <v>215</v>
-      </c>
-      <c r="F24" s="33">
-        <v>41710</v>
-      </c>
-      <c r="G24" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="H24" s="17">
-        <v>41712</v>
-      </c>
-      <c r="I24" t="s">
-        <v>216</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" topLeftCell="B1">
+      <selection activeCell="H24" sqref="H24"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
       <selection activeCell="E24" sqref="E24"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" topLeftCell="B1">
-      <selection activeCell="H24" sqref="H24"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
   </customSheetViews>
   <mergeCells count="11">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A5:A8"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A19:A20"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A5:A8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
@@ -3232,137 +3380,143 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E8:E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.83203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="9"/>
+    <col min="1" max="1" width="39.6640625" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" style="43" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.83203125" style="8" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="15" customFormat="1">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:10" s="13" customFormat="1">
+      <c r="A1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="15" t="s">
+      <c r="C1" s="35"/>
+      <c r="D1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="37"/>
+      <c r="H1" s="35"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="9">
         <v>41690</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="43">
         <v>41691</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="9">
         <v>41694</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>80</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="9">
         <v>41694</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="8" t="s">
         <v>78</v>
+      </c>
+      <c r="G4" s="43">
+        <v>41732</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>84</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <v>41700</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="38"/>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>96</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -3370,56 +3524,62 @@
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>88</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>41700</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="8" t="s">
         <v>78</v>
       </c>
+      <c r="G7" s="43">
+        <v>41734</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>90</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
         <v>41708</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="8" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="D9" s="32"/>
-      <c r="E9" s="10">
+      <c r="D9" s="30"/>
+      <c r="E9" s="9">
         <v>41723</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" t="s">
+      <c r="A10" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>151</v>
       </c>
       <c r="C10" t="s">
@@ -3428,104 +3588,103 @@
       <c r="D10" t="s">
         <v>153</v>
       </c>
-      <c r="E10" s="31">
+      <c r="E10" s="29">
         <v>41711</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="G10" s="28">
+      <c r="G10" s="44">
         <v>41716</v>
       </c>
-      <c r="H10" s="17" t="s">
-        <v>209</v>
-      </c>
-      <c r="I10" t="s">
-        <v>208</v>
+      <c r="H10" t="s">
+        <v>227</v>
       </c>
       <c r="J10"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>104</v>
       </c>
       <c r="D12" t="s">
         <v>105</v>
       </c>
-      <c r="E12" s="28">
+      <c r="E12" s="26">
         <v>41711</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G12" s="17"/>
-      <c r="H12"/>
+      <c r="G12" s="44"/>
+      <c r="H12" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="B15" s="9" t="s">
+      <c r="A15" s="34" t="s">
+        <v>216</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="E15" s="10">
+      <c r="E15" s="9">
         <v>41718</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="8" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="E16" s="10">
+      <c r="E16" s="9">
         <v>41723</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="8" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="34" t="s">
+        <v>220</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="C17" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="D17" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="E17" s="10">
+      <c r="E17" s="9">
         <v>41721</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="8" t="s">
         <v>78</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
+      <selection activeCell="G14" sqref="G14"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" topLeftCell="B1">
       <selection activeCell="F14" sqref="F14"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
-      <selection activeCell="F7" sqref="F7"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
@@ -3569,27 +3728,27 @@
     <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="15" customFormat="1">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:8" s="13" customFormat="1">
+      <c r="A1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="15" t="s">
+      <c r="C1" s="35"/>
+      <c r="D1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="37"/>
+      <c r="H1" s="35"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="39" t="s">
@@ -3604,7 +3763,7 @@
       <c r="D2" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="15">
         <v>41690</v>
       </c>
       <c r="F2" s="39" t="s">
@@ -3616,18 +3775,18 @@
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
       <c r="D3" s="40"/>
-      <c r="E3" s="17">
+      <c r="E3" s="15">
         <v>41718</v>
       </c>
       <c r="F3" s="39"/>
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
+      <selection activeCell="F2" sqref="F2:F3"/>
+    </customSheetView>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
       <selection activeCell="E3" sqref="E3"/>
-    </customSheetView>
-    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
-      <selection activeCell="F2" sqref="F2:F3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="7">
@@ -3670,20 +3829,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="26" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="24" t="s">
         <v>206</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="25" t="s">
         <v>207</v>
       </c>
     </row>
@@ -3714,7 +3873,7 @@
       <c r="E3" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="15">
         <v>41711</v>
       </c>
       <c r="G3" t="s">
@@ -3773,7 +3932,7 @@
       <c r="E7" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="15">
         <v>41711</v>
       </c>
       <c r="G7" t="s">
@@ -3888,13 +4047,13 @@
       <c r="E15" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="15">
         <v>41711</v>
       </c>
       <c r="G15" t="s">
         <v>78</v>
       </c>
-      <c r="H15" s="17">
+      <c r="H15" s="15">
         <v>41716</v>
       </c>
       <c r="I15" t="s">
@@ -3955,12 +4114,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
+      <selection activeCell="C16" sqref="C16"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
       <selection activeCell="C7" sqref="C7"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
-      <selection activeCell="C16" sqref="C16"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
@@ -4001,7 +4160,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4014,20 +4173,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="17" t="s">
         <v>66</v>
       </c>
       <c r="B1" s="41" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="41"/>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="18" t="s">
         <v>69</v>
       </c>
       <c r="G1" s="41" t="s">
@@ -4042,7 +4201,7 @@
       <c r="B2" s="42" t="s">
         <v>168</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="20" t="s">
         <v>166</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -4052,13 +4211,13 @@
     <row r="3" spans="1:8">
       <c r="A3" s="42"/>
       <c r="B3" s="42"/>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="22" t="s">
         <v>201</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="26">
         <v>41717</v>
       </c>
       <c r="F3" t="s">
@@ -4067,16 +4226,16 @@
     </row>
     <row r="4" spans="1:8" ht="36">
       <c r="A4" s="42"/>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="23" t="s">
         <v>204</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="22" t="s">
         <v>203</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="26">
         <v>41717</v>
       </c>
       <c r="F4" t="s">
@@ -4088,13 +4247,13 @@
       <c r="B5" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="22" t="s">
         <v>199</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="15">
         <v>41718</v>
       </c>
       <c r="F5" t="s">
@@ -4104,7 +4263,7 @@
     <row r="6" spans="1:8">
       <c r="A6" s="42"/>
       <c r="B6" s="39"/>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="20" t="s">
         <v>169</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -4112,30 +4271,30 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="21" t="s">
         <v>174</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="26">
         <v>41711</v>
       </c>
       <c r="F7" t="s">
         <v>78</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="15">
         <v>41723</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="20" t="s">
         <v>176</v>
       </c>
       <c r="B8" t="s">
@@ -4147,7 +4306,7 @@
       <c r="D8" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8" s="26">
         <v>41711</v>
       </c>
       <c r="F8" t="s">
@@ -4155,7 +4314,7 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="20" t="s">
         <v>180</v>
       </c>
       <c r="B9" t="s">
@@ -4167,7 +4326,7 @@
       <c r="D9" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E9" s="26">
         <v>41717</v>
       </c>
       <c r="F9" t="s">
@@ -4175,7 +4334,7 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="20" t="s">
         <v>129</v>
       </c>
       <c r="B10" t="s">
@@ -4187,7 +4346,7 @@
       <c r="D10" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10" s="26">
         <v>41346</v>
       </c>
       <c r="F10" t="s">
@@ -4195,7 +4354,7 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="20" t="s">
         <v>183</v>
       </c>
       <c r="B11" t="s">
@@ -4207,7 +4366,7 @@
       <c r="D11" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E11" s="26">
         <v>41717</v>
       </c>
       <c r="F11" t="s">
@@ -4215,7 +4374,7 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="20" t="s">
         <v>187</v>
       </c>
       <c r="B12" t="s">
@@ -4227,7 +4386,7 @@
       <c r="D12" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E12" s="28">
+      <c r="E12" s="26">
         <v>41711</v>
       </c>
       <c r="F12" t="s">
@@ -4235,14 +4394,14 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="22"/>
+      <c r="A13" s="20"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="28">
+      <c r="E13" s="26">
         <v>41723</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="20" t="s">
         <v>188</v>
       </c>
       <c r="B14" t="s">
@@ -4254,7 +4413,7 @@
       <c r="D14" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="E14" s="28">
+      <c r="E14" s="26">
         <v>41717</v>
       </c>
       <c r="F14" t="s">
@@ -4262,7 +4421,7 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="20" t="s">
         <v>192</v>
       </c>
       <c r="B15" t="s">
@@ -4276,7 +4435,7 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="20" t="s">
         <v>195</v>
       </c>
       <c r="B16" t="s">
@@ -4290,8 +4449,8 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="22" t="s">
-        <v>211</v>
+      <c r="A17" s="20" t="s">
+        <v>210</v>
       </c>
       <c r="B17" t="s">
         <v>87</v>
@@ -4302,7 +4461,7 @@
       <c r="D17" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E17" s="28">
+      <c r="E17" s="26">
         <v>41711</v>
       </c>
       <c r="F17" t="s">
@@ -4310,30 +4469,30 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="E18" s="17">
+      <c r="E18" s="15">
         <v>41723</v>
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="B19" t="s">
         <v>217</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>218</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>219</v>
       </c>
-      <c r="D19" t="s">
-        <v>220</v>
-      </c>
-      <c r="E19" s="34">
+      <c r="E19" s="32">
         <v>41718</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B24" t="s">
         <v>151</v>
@@ -4344,13 +4503,13 @@
       <c r="D24" t="s">
         <v>153</v>
       </c>
-      <c r="E24" s="28">
+      <c r="E24" s="26">
         <v>41711</v>
       </c>
       <c r="F24" t="s">
         <v>78</v>
       </c>
-      <c r="G24" s="28">
+      <c r="G24" s="26">
         <v>41716</v>
       </c>
       <c r="H24" t="s">
@@ -4359,11 +4518,11 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
+      <selection activeCell="D18" sqref="D18"/>
+    </customSheetView>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
       <selection activeCell="F8" sqref="F8"/>
-    </customSheetView>
-    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
-      <selection activeCell="D18" sqref="D18"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="5">
@@ -4407,8 +4566,8 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
   <customSheetViews>
+    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}"/>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}"/>
-    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}"/>
   </customSheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
updates to the list of responses
git-svn-id: svn+ssh://svn.cern.ch/reps/jansvn/trunk/lcDetRnD@526 4525493e-7705-40b1-a816-d608a930855b
</commit_message>
<xml_diff>
--- a/ListOfGroups.xlsx
+++ b/ListOfGroups.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="0" windowWidth="28720" windowHeight="17380" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-40" yWindow="0" windowWidth="28720" windowHeight="17380" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TPC" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Jan Strube - Personal View" guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" mergeInterval="0" personalView="1" xWindow="-2" yWindow="54" windowWidth="1436" windowHeight="815" tabRatio="500" activeSheetId="2"/>
+    <customWorkbookView name="Jan Strube - Personal View" guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" mergeInterval="0" personalView="1" xWindow="-2" yWindow="54" windowWidth="1436" windowHeight="815" tabRatio="500" activeSheetId="5"/>
     <customWorkbookView name="TITOV Maksym - Personal View" guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1243" windowHeight="652" tabRatio="500" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="234">
   <si>
     <t>Leader</t>
   </si>
@@ -338,9 +338,6 @@
   </si>
   <si>
     <t>kriles@umich.edu</t>
-  </si>
-  <si>
-    <t>Silicon Development</t>
   </si>
   <si>
     <t>Bruce Schumm</t>
@@ -758,6 +755,21 @@
   </si>
   <si>
     <t>Tracker_SCIPPTracking_BruceSchumm_SCIPP_20140326.docx</t>
+  </si>
+  <si>
+    <t>CLICPix_LucieLinssen_CERN_20140404.pdf</t>
+  </si>
+  <si>
+    <t>Marcel Vos</t>
+  </si>
+  <si>
+    <t>marcel.vos@cern.ch</t>
+  </si>
+  <si>
+    <t>FCAL_WolfgangLohmann_DESY_20140327.pdf</t>
+  </si>
+  <si>
+    <t>FCAL_WolfgangLohmann_DESY_20140327.tar</t>
   </si>
 </sst>
 </file>
@@ -845,9 +857,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -967,12 +980,13 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -987,7 +1001,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{FAE6AD53-8B02-964B-9E03-2DA6A505E01F}" diskRevisions="1" revisionId="113" version="4">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{4101B9EF-F6AE-5D4D-9600-DC73FEFB3B43}" diskRevisions="1" revisionId="128" version="5">
   <header guid="{90EFB229-A129-4641-96FB-C4C9036C70D7}" dateTime="2014-03-18T10:37:43" maxSheetId="6" userName="Jan Strube" r:id="rId1">
     <sheetIdMap count="5">
       <sheetId val="1"/>
@@ -1210,6 +1224,17 @@
       <sheetId val="7"/>
     </sheetIdMap>
   </header>
+  <header guid="{4101B9EF-F6AE-5D4D-9600-DC73FEFB3B43}" dateTime="2014-04-05T13:50:08" maxSheetId="8" userName="Jan Strube" r:id="rId24" minRId="114" maxRId="128">
+    <sheetIdMap count="7">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -2228,6 +2253,256 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog24.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="114" sId="2" numFmtId="19">
+    <nc r="G12">
+      <v>41724</v>
+    </nc>
+  </rcc>
+  <rcc rId="115" sId="2" xfDxf="1" dxf="1">
+    <nc r="H15" t="inlineStr">
+      <is>
+        <t>CLICPix_LucieLinssen_CERN_20140404.pdf</t>
+      </is>
+    </nc>
+    <ndxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="116" sId="2" numFmtId="19">
+    <nc r="G15">
+      <v>41733</v>
+    </nc>
+  </rcc>
+  <rrc rId="117" sId="2" ref="A4:XFD4" action="insertRow"/>
+  <rcc rId="118" sId="2">
+    <nc r="C4" t="inlineStr">
+      <is>
+        <t>Marcel Vos</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="119" sId="2">
+    <nc r="D4" t="inlineStr">
+      <is>
+        <t>marcel.vos@cern.ch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="120" sId="2">
+    <nc r="C19" t="inlineStr">
+      <is>
+        <t>Marcel Vos</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="121" sId="2" odxf="1" s="1" dxf="1">
+    <nc r="D19" t="inlineStr">
+      <is>
+        <t>marcel.vos@cern.ch</t>
+      </is>
+    </nc>
+    <odxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </odxf>
+    <ndxf>
+      <font>
+        <u/>
+        <sz val="12"/>
+        <color theme="10"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </ndxf>
+  </rcc>
+  <rrc rId="122" sId="4" ref="A15:XFD15" action="deleteRow">
+    <rfmt sheetId="4" xfDxf="1" sqref="A15:XFD15" start="0" length="0"/>
+    <rcc rId="0" sId="4">
+      <nc r="A15" t="inlineStr">
+        <is>
+          <t>Kpix</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="4">
+      <nc r="C15" t="inlineStr">
+        <is>
+          <t>SLAC</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="4">
+      <nc r="D15" t="inlineStr">
+        <is>
+          <t>Marty Breidenbach</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="4" s="1" dxf="1">
+      <nc r="E15" t="inlineStr">
+        <is>
+          <t>mib@slac.stanford.edu</t>
+        </is>
+      </nc>
+      <ndxf>
+        <font>
+          <u/>
+          <sz val="12"/>
+          <color theme="10"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="4" dxf="1" numFmtId="21">
+      <nc r="F15">
+        <v>41711</v>
+      </nc>
+      <ndxf>
+        <numFmt numFmtId="21" formatCode="d\-mmm"/>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="4">
+      <nc r="G15" t="inlineStr">
+        <is>
+          <t>Jan</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="4" dxf="1" numFmtId="21">
+      <nc r="H15">
+        <v>41716</v>
+      </nc>
+      <ndxf>
+        <numFmt numFmtId="21" formatCode="d\-mmm"/>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="4">
+      <nc r="I15" t="inlineStr">
+        <is>
+          <t>KPiX_RD_Status.docx</t>
+        </is>
+      </nc>
+    </rcc>
+  </rrc>
+  <rrc rId="123" sId="4" ref="A3:XFD3" action="deleteRow">
+    <rfmt sheetId="4" xfDxf="1" sqref="A3:XFD3" start="0" length="0"/>
+    <rcc rId="0" sId="4">
+      <nc r="A3" t="inlineStr">
+        <is>
+          <t>Silicon Development</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="4">
+      <nc r="C3" t="inlineStr">
+        <is>
+          <t>SCIPP, UCSC</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="4">
+      <nc r="D3" t="inlineStr">
+        <is>
+          <t>Bruce Schumm</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="4" s="1" dxf="1">
+      <nc r="E3" t="inlineStr">
+        <is>
+          <t>schumm@scipp.ucsc.edu</t>
+        </is>
+      </nc>
+      <ndxf>
+        <font>
+          <u/>
+          <sz val="12"/>
+          <color theme="10"/>
+          <name val="Calibri"/>
+          <scheme val="minor"/>
+        </font>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="4" dxf="1" numFmtId="21">
+      <nc r="F3">
+        <v>41711</v>
+      </nc>
+      <ndxf>
+        <numFmt numFmtId="21" formatCode="d\-mmm"/>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="4">
+      <nc r="G3" t="inlineStr">
+        <is>
+          <t>Jan</t>
+        </is>
+      </nc>
+    </rcc>
+  </rrc>
+  <rfmt sheetId="3" sqref="G3" start="0" length="0">
+    <dxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="124" sId="3" xfDxf="1" dxf="1">
+    <nc r="H3" t="inlineStr">
+      <is>
+        <t>FCAL_WolfgangLohmann_DESY_20140327.pdf</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="125" sId="3" xfDxf="1" dxf="1">
+    <nc r="H4" t="inlineStr">
+      <is>
+        <t>FCAL_WolfgangLohmann_DESY_20140327.tar</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="126" sId="3" numFmtId="21">
+    <nc r="G3">
+      <v>41725</v>
+    </nc>
+  </rcc>
+  <rcc rId="127" sId="5">
+    <nc r="F19" t="inlineStr">
+      <is>
+        <t>Jan</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="128" sId="5" odxf="1" dxf="1" numFmtId="21">
+    <nc r="G19">
+      <v>41733</v>
+    </nc>
+    <odxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </odxf>
+    <ndxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </ndxf>
+  </rcc>
+  <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="delete"/>
+  <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="12" sId="5" odxf="1" dxf="1" numFmtId="19">
@@ -2650,9 +2925,7 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
-  <userInfo guid="{FAE6AD53-8B02-964B-9E03-2DA6A505E01F}" name="Jan Strube" id="-985427944" dateTime="2014-04-05T13:05:11"/>
-</users>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2980,7 +3253,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3302,10 +3575,10 @@
         <v>29</v>
       </c>
       <c r="D24" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="E24" s="28" t="s">
         <v>213</v>
-      </c>
-      <c r="E24" s="28" t="s">
-        <v>214</v>
       </c>
       <c r="F24" s="31">
         <v>41710</v>
@@ -3317,13 +3590,13 @@
         <v>41712</v>
       </c>
       <c r="I24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" topLeftCell="B1">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="H22" sqref="H22"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
@@ -3378,10 +3651,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3466,221 +3739,245 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="34" t="s">
+      <c r="C4" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C5" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E5" s="9">
         <v>41694</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="G4" s="43">
-        <v>41732</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E5" s="9">
-        <v>41700</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>78</v>
       </c>
+      <c r="G5" s="43">
+        <v>41732</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="38"/>
+      <c r="A6" s="38" t="s">
+        <v>82</v>
+      </c>
       <c r="B6" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="9">
+        <v>41700</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="38"/>
+      <c r="B7" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C7" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="E7" s="9">
-        <v>41700</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="G7" s="43">
-        <v>41734</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="34" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>8</v>
+        <v>87</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
       <c r="E8" s="9">
-        <v>41708</v>
+        <v>41700</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>78</v>
       </c>
+      <c r="G8" s="43">
+        <v>41734</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="D9" s="30"/>
+      <c r="A9" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>91</v>
+      </c>
       <c r="E9" s="9">
+        <v>41708</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="D10" s="30"/>
+      <c r="E10" s="9">
         <v>41723</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="33" t="s">
+    <row r="11" spans="1:10">
+      <c r="A11" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="C11" t="s">
         <v>151</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D11" t="s">
         <v>152</v>
       </c>
-      <c r="D10" t="s">
-        <v>153</v>
-      </c>
-      <c r="E10" s="29">
+      <c r="E11" s="29">
         <v>41711</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F11" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="G10" s="44">
+      <c r="G11" s="44">
         <v>41716</v>
       </c>
-      <c r="H10" t="s">
-        <v>227</v>
-      </c>
-      <c r="J10"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="B12" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="C12" s="8" t="s">
+      <c r="H11" t="s">
+        <v>226</v>
+      </c>
+      <c r="J11"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="B13" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" t="s">
         <v>104</v>
       </c>
-      <c r="D12" t="s">
-        <v>105</v>
-      </c>
-      <c r="E12" s="26">
+      <c r="E13" s="26">
         <v>41711</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G12" s="44"/>
-      <c r="H12" t="s">
+      <c r="G13" s="44">
+        <v>41724</v>
+      </c>
+      <c r="H13" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="E16" s="9">
+        <v>41718</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" s="43">
+        <v>41733</v>
+      </c>
+      <c r="H16" s="8" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="34" t="s">
-        <v>216</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="E15" s="9">
-        <v>41718</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="C16" s="8" t="s">
+    <row r="17" spans="1:6">
+      <c r="C17" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="E16" s="9">
+      <c r="E17" s="9">
         <v>41723</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="34" t="s">
-        <v>220</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="E17" s="9">
-        <v>41721</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="34" t="s">
+        <v>219</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="E18" s="9">
+        <v>41721</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="C19" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E20" sqref="E20"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" topLeftCell="B1">
@@ -3691,15 +3988,15 @@
   <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A6:A7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
     <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
-    <hyperlink ref="D8" r:id="rId5"/>
-    <hyperlink ref="D6" r:id="rId6"/>
+    <hyperlink ref="D5" r:id="rId3"/>
+    <hyperlink ref="D6" r:id="rId4"/>
+    <hyperlink ref="D9" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3713,10 +4010,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3779,11 +4076,22 @@
         <v>41718</v>
       </c>
       <c r="F3" s="39"/>
+      <c r="G3" s="15">
+        <v>41725</v>
+      </c>
+      <c r="H3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="H4" t="s">
+        <v>233</v>
+      </c>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
-      <selection activeCell="F2" sqref="F2:F3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </customSheetView>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
       <selection activeCell="E3" sqref="E3"/>
@@ -3812,10 +4120,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3828,7 +4136,7 @@
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" s="16" t="s">
         <v>98</v>
       </c>
@@ -3837,16 +4145,16 @@
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
       <c r="F1" s="24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G1" s="25" t="s">
         <v>69</v>
       </c>
       <c r="H1" s="25" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -3860,160 +4168,152 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D3" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F3" s="15">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="C6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F6" s="15">
         <v>41711</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D4" t="s">
-        <v>109</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D5" t="s">
-        <v>113</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D6" t="s">
-        <v>116</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>124</v>
+      </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="D7" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F7" s="15">
-        <v>41711</v>
-      </c>
-      <c r="G7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
-        <v>125</v>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="39" t="s">
+        <v>128</v>
       </c>
       <c r="C8" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D8" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="39" t="s">
-        <v>129</v>
-      </c>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="39"/>
       <c r="C9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D9" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="39"/>
+      <c r="B10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D11" t="s">
+        <v>140</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="39"/>
-      <c r="C10" t="s">
-        <v>133</v>
-      </c>
-      <c r="D10" t="s">
-        <v>134</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="39"/>
-      <c r="B11" t="s">
-        <v>139</v>
-      </c>
-      <c r="C11" t="s">
-        <v>137</v>
-      </c>
-      <c r="D11" t="s">
-        <v>136</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
-        <v>140</v>
-      </c>
-      <c r="C12" t="s">
-        <v>143</v>
-      </c>
       <c r="D12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="39" t="s">
-        <v>144</v>
-      </c>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="39"/>
       <c r="C13" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="D13" t="s">
         <v>145</v>
@@ -4022,100 +4322,62 @@
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="39"/>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>153</v>
+      </c>
       <c r="C14" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="D14" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" t="s">
-        <v>150</v>
-      </c>
-      <c r="C15" t="s">
-        <v>151</v>
-      </c>
-      <c r="D15" t="s">
-        <v>152</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="F15" s="15">
-        <v>41711</v>
-      </c>
-      <c r="G15" t="s">
-        <v>78</v>
-      </c>
-      <c r="H15" s="15">
-        <v>41716</v>
-      </c>
-      <c r="I15" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" t="s">
-        <v>154</v>
-      </c>
-      <c r="C16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="39" t="s">
         <v>157</v>
       </c>
+      <c r="B16" s="39"/>
       <c r="D16" t="s">
-        <v>155</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>156</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="39"/>
+      <c r="B17" s="39"/>
+      <c r="D17" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="39" t="s">
-        <v>158</v>
-      </c>
+      <c r="A18" s="39"/>
       <c r="B18" s="39"/>
       <c r="D18" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="39"/>
       <c r="B19" s="39"/>
       <c r="D19" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="39"/>
-      <c r="B20" s="39"/>
+      <c r="A20" t="s">
+        <v>158</v>
+      </c>
       <c r="D20" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="39"/>
-      <c r="B21" s="39"/>
-      <c r="D21" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
         <v>159</v>
-      </c>
-      <c r="D22" t="s">
-        <v>160</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
@@ -4124,9 +4386,9 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="3">
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A18:B21"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A16:B19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
@@ -4142,8 +4404,6 @@
     <hyperlink ref="E12" r:id="rId11"/>
     <hyperlink ref="E13" r:id="rId12"/>
     <hyperlink ref="E14" r:id="rId13"/>
-    <hyperlink ref="E15" r:id="rId14"/>
-    <hyperlink ref="E16" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4159,8 +4419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4196,26 +4456,26 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="B2" s="42" t="s">
-        <v>168</v>
-      </c>
-      <c r="C2" s="20" t="s">
+      <c r="D2" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="42"/>
       <c r="B3" s="42"/>
       <c r="C3" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="E3" s="26">
         <v>41717</v>
@@ -4227,13 +4487,13 @@
     <row r="4" spans="1:8" ht="36">
       <c r="A4" s="42"/>
       <c r="B4" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>203</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>205</v>
       </c>
       <c r="E4" s="26">
         <v>41717</v>
@@ -4245,13 +4505,13 @@
     <row r="5" spans="1:8">
       <c r="A5" s="42"/>
       <c r="B5" s="39" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C5" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>200</v>
       </c>
       <c r="E5" s="15">
         <v>41718</v>
@@ -4264,24 +4524,24 @@
       <c r="A6" s="42"/>
       <c r="B6" s="39"/>
       <c r="C6" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="C7" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="D7" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="E7" s="26">
         <v>41711</v>
@@ -4295,16 +4555,16 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" t="s">
         <v>176</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>177</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="E8" s="26">
         <v>41711</v>
@@ -4315,16 +4575,16 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B9" t="s">
         <v>45</v>
       </c>
       <c r="C9" t="s">
+        <v>180</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="E9" s="26">
         <v>41717</v>
@@ -4335,16 +4595,16 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C10" t="s">
         <v>129</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="C10" t="s">
-        <v>130</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="E10" s="26">
         <v>41346</v>
@@ -4355,16 +4615,16 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="B11" t="s">
         <v>183</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
+        <v>185</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="C11" t="s">
-        <v>186</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="E11" s="26">
         <v>41717</v>
@@ -4375,16 +4635,16 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="C12" t="s">
-        <v>122</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="E12" s="26">
         <v>41711</v>
@@ -4402,16 +4662,16 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="B14" t="s">
         <v>188</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>189</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="E14" s="26">
         <v>41717</v>
@@ -4422,44 +4682,44 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B15" t="s">
         <v>62</v>
       </c>
       <c r="C15" t="s">
+        <v>192</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="B16" t="s">
+        <v>196</v>
+      </c>
+      <c r="C16" t="s">
         <v>195</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="C16" t="s">
-        <v>196</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B17" t="s">
         <v>87</v>
       </c>
       <c r="C17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E17" s="26">
         <v>41711</v>
@@ -4475,33 +4735,39 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="B19" t="s">
         <v>216</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>217</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>218</v>
-      </c>
-      <c r="D19" t="s">
-        <v>219</v>
       </c>
       <c r="E19" s="32">
         <v>41718</v>
       </c>
+      <c r="F19" t="s">
+        <v>78</v>
+      </c>
+      <c r="G19" s="15">
+        <v>41733</v>
+      </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B24" t="s">
+        <v>150</v>
+      </c>
+      <c r="C24" t="s">
         <v>151</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>152</v>
-      </c>
-      <c r="D24" t="s">
-        <v>153</v>
       </c>
       <c r="E24" s="26">
         <v>41711</v>
@@ -4513,13 +4779,13 @@
         <v>41716</v>
       </c>
       <c r="H24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="G11" sqref="G11"/>
     </customSheetView>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
       <selection activeCell="F8" sqref="F8"/>

</xml_diff>

<commit_message>
update to list of groups
git-svn-id: svn+ssh://svn.cern.ch/reps/jansvn/trunk/lcDetRnD@529 4525493e-7705-40b1-a816-d608a930855b
</commit_message>
<xml_diff>
--- a/ListOfGroups.xlsx
+++ b/ListOfGroups.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="236">
   <si>
     <t>Leader</t>
   </si>
@@ -770,6 +770,12 @@
   </si>
   <si>
     <t>FCAL_WolfgangLohmann_DESY_20140327.tar</t>
+  </si>
+  <si>
+    <t>CERN_LCDGroup_LucieLinssen_CERN_20140404.pdf</t>
+  </si>
+  <si>
+    <t>GEM_DHCAL_AndyWhite_UTA_20140326.doc</t>
   </si>
 </sst>
 </file>
@@ -857,9 +863,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -953,14 +960,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -977,16 +986,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1001,7 +1009,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{4101B9EF-F6AE-5D4D-9600-DC73FEFB3B43}" diskRevisions="1" revisionId="128" version="5">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{E10FDDBA-7369-7F46-9E10-0216F9A48312}" diskRevisions="1" revisionId="132" version="7">
   <header guid="{90EFB229-A129-4641-96FB-C4C9036C70D7}" dateTime="2014-03-18T10:37:43" maxSheetId="6" userName="Jan Strube" r:id="rId1">
     <sheetIdMap count="5">
       <sheetId val="1"/>
@@ -1235,6 +1243,28 @@
       <sheetId val="7"/>
     </sheetIdMap>
   </header>
+  <header guid="{97119F5E-1AE8-DD4E-A39E-4B9FDBC962E5}" dateTime="2014-04-06T23:07:02" maxSheetId="8" userName="Jan Strube" r:id="rId25" minRId="129" maxRId="131">
+    <sheetIdMap count="7">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{E10FDDBA-7369-7F46-9E10-0216F9A48312}" dateTime="2014-04-06T23:07:54" maxSheetId="8" userName="Jan Strube" r:id="rId26" minRId="132">
+    <sheetIdMap count="7">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -2503,6 +2533,44 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog25.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="129" sId="5" xfDxf="1" dxf="1">
+    <nc r="H19" t="inlineStr">
+      <is>
+        <t>CERN_LCDGroup_LucieLinssen_CERN_20140404.pdf</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="130" sId="5" xfDxf="1" dxf="1">
+    <nc r="H12" t="inlineStr">
+      <is>
+        <t>GEM_DHCAL_AndyWhite_UTA_20140326.doc</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="131" sId="5" odxf="1" dxf="1" numFmtId="21">
+    <nc r="G12">
+      <v>41724</v>
+    </nc>
+    <odxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </odxf>
+    <ndxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </ndxf>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog26.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rm rId="132" sheetId="5" source="A15:D15" destination="A20:D20" sourceSheetId="5"/>
+  <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="delete"/>
+  <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="12" sId="5" odxf="1" dxf="1" numFmtId="19">
@@ -2925,7 +2993,9 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+  <userInfo guid="{E10FDDBA-7369-7F46-9E10-0216F9A48312}" name="Jan Strube" id="-985401621" dateTime="2014-04-06T23:03:40"/>
+</users>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3276,10 +3346,10 @@
       <c r="B1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="35"/>
+      <c r="D1" s="39"/>
       <c r="E1" s="13" t="s">
         <v>1</v>
       </c>
@@ -3298,7 +3368,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="38" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -3311,7 +3381,7 @@
     <row r="3" spans="1:8">
       <c r="A3" s="37"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="36"/>
+      <c r="C3" s="38"/>
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
@@ -3409,7 +3479,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="37"/>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="38" t="s">
         <v>30</v>
       </c>
       <c r="D10" t="s">
@@ -3421,7 +3491,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="37"/>
-      <c r="C11" s="36"/>
+      <c r="C11" s="38"/>
       <c r="D11" t="s">
         <v>35</v>
       </c>
@@ -3605,17 +3675,17 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="11">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A5:A8"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A19:A20"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A5:A8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
@@ -3654,7 +3724,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3665,7 +3735,7 @@
     <col min="4" max="4" width="25.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" style="43" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" style="35" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="51.83203125" style="8" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="8"/>
   </cols>
@@ -3674,10 +3744,10 @@
       <c r="A1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="35"/>
+      <c r="C1" s="39"/>
       <c r="D1" s="13" t="s">
         <v>1</v>
       </c>
@@ -3687,10 +3757,10 @@
       <c r="F1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="35"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="34" t="s">
@@ -3711,7 +3781,7 @@
       <c r="F2" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="43">
+      <c r="G2" s="35">
         <v>41691</v>
       </c>
       <c r="H2" s="8" t="s">
@@ -3765,7 +3835,7 @@
       <c r="F5" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="G5" s="43">
+      <c r="G5" s="35">
         <v>41732</v>
       </c>
       <c r="H5" s="8" t="s">
@@ -3773,7 +3843,7 @@
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="40" t="s">
         <v>82</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -3793,7 +3863,7 @@
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="38"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="8" t="s">
         <v>52</v>
       </c>
@@ -3823,7 +3893,7 @@
       <c r="F8" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="G8" s="43">
+      <c r="G8" s="35">
         <v>41734</v>
       </c>
       <c r="H8" s="8" t="s">
@@ -3875,7 +3945,7 @@
       <c r="F11" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="G11" s="44">
+      <c r="G11" s="36">
         <v>41716</v>
       </c>
       <c r="H11" t="s">
@@ -3899,7 +3969,7 @@
       <c r="F13" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G13" s="44">
+      <c r="G13" s="36">
         <v>41724</v>
       </c>
       <c r="H13" t="s">
@@ -3925,7 +3995,7 @@
       <c r="F16" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="G16" s="43">
+      <c r="G16" s="35">
         <v>41733</v>
       </c>
       <c r="H16" s="8" t="s">
@@ -3977,7 +4047,7 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="H16" sqref="H16"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" topLeftCell="B1">
@@ -4029,10 +4099,10 @@
       <c r="A1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="35"/>
+      <c r="C1" s="39"/>
       <c r="D1" s="13" t="s">
         <v>1</v>
       </c>
@@ -4042,40 +4112,40 @@
       <c r="F1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="35"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="42" t="s">
         <v>95</v>
       </c>
       <c r="E2" s="15">
         <v>41690</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="41" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="39"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="40"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="42"/>
       <c r="E3" s="15">
         <v>41718</v>
       </c>
-      <c r="F3" s="39"/>
+      <c r="F3" s="41"/>
       <c r="G3" s="15">
         <v>41725</v>
       </c>
@@ -4242,7 +4312,7 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="41" t="s">
         <v>128</v>
       </c>
       <c r="C8" t="s">
@@ -4256,7 +4326,7 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="39"/>
+      <c r="A9" s="41"/>
       <c r="C9" t="s">
         <v>132</v>
       </c>
@@ -4268,7 +4338,7 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="39"/>
+      <c r="A10" s="41"/>
       <c r="B10" t="s">
         <v>138</v>
       </c>
@@ -4297,7 +4367,7 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="41" t="s">
         <v>143</v>
       </c>
       <c r="C12" t="s">
@@ -4311,7 +4381,7 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="39"/>
+      <c r="A13" s="41"/>
       <c r="C13" t="s">
         <v>146</v>
       </c>
@@ -4337,31 +4407,31 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="41" t="s">
         <v>157</v>
       </c>
-      <c r="B16" s="39"/>
+      <c r="B16" s="41"/>
       <c r="D16" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="39"/>
-      <c r="B17" s="39"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="41"/>
       <c r="D17" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="39"/>
-      <c r="B18" s="39"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="41"/>
       <c r="D18" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="39"/>
-      <c r="B19" s="39"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="D19" t="s">
         <v>163</v>
       </c>
@@ -4420,7 +4490,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4436,10 +4506,10 @@
       <c r="A1" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="41"/>
+      <c r="C1" s="43"/>
       <c r="D1" s="18" t="s">
         <v>1</v>
       </c>
@@ -4449,16 +4519,16 @@
       <c r="F1" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="41"/>
+      <c r="H1" s="43"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="44" t="s">
         <v>164</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="44" t="s">
         <v>167</v>
       </c>
       <c r="C2" s="20" t="s">
@@ -4469,8 +4539,8 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="42"/>
-      <c r="B3" s="42"/>
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
       <c r="C3" s="22" t="s">
         <v>200</v>
       </c>
@@ -4485,7 +4555,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="36">
-      <c r="A4" s="42"/>
+      <c r="A4" s="44"/>
       <c r="B4" s="23" t="s">
         <v>203</v>
       </c>
@@ -4503,8 +4573,8 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="42"/>
-      <c r="B5" s="39" t="s">
+      <c r="A5" s="44"/>
+      <c r="B5" s="41" t="s">
         <v>170</v>
       </c>
       <c r="C5" s="22" t="s">
@@ -4521,8 +4591,8 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="42"/>
-      <c r="B6" s="39"/>
+      <c r="A6" s="44"/>
+      <c r="B6" s="41"/>
       <c r="C6" s="20" t="s">
         <v>168</v>
       </c>
@@ -4651,6 +4721,12 @@
       </c>
       <c r="F12" t="s">
         <v>78</v>
+      </c>
+      <c r="G12" s="15">
+        <v>41724</v>
+      </c>
+      <c r="H12" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -4680,20 +4756,6 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="20" t="s">
-        <v>191</v>
-      </c>
-      <c r="B15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" t="s">
-        <v>192</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
     <row r="16" spans="1:8">
       <c r="A16" s="20" t="s">
         <v>194</v>
@@ -4755,6 +4817,23 @@
       <c r="G19" s="15">
         <v>41733</v>
       </c>
+      <c r="H19" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" t="s">
+        <v>192</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
@@ -4785,7 +4864,8 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G20" sqref="G20"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
       <selection activeCell="F8" sqref="F8"/>
@@ -4808,13 +4888,14 @@
     <hyperlink ref="D11" r:id="rId7"/>
     <hyperlink ref="D12" r:id="rId8"/>
     <hyperlink ref="D14" r:id="rId9"/>
-    <hyperlink ref="D15" r:id="rId10"/>
+    <hyperlink ref="D20" r:id="rId10"/>
     <hyperlink ref="D16" r:id="rId11"/>
     <hyperlink ref="D5" r:id="rId12"/>
     <hyperlink ref="D3" r:id="rId13"/>
     <hyperlink ref="D4" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Adding contributions from Felix Sefkow on the AHCAL
git-svn-id: svn+ssh://svn.cern.ch/reps/jansvn/trunk/lcDetRnD@533 4525493e-7705-40b1-a816-d608a930855b
</commit_message>
<xml_diff>
--- a/ListOfGroups.xlsx
+++ b/ListOfGroups.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="0" windowWidth="28720" windowHeight="17380" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-40" yWindow="0" windowWidth="28720" windowHeight="17380" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TPC" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,8 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jan Strube - Personal View" guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" mergeInterval="0" personalView="1" xWindow="-2" yWindow="54" windowWidth="1436" windowHeight="815" tabRatio="500" activeSheetId="5"/>
     <customWorkbookView name="TITOV Maksym - Personal View" guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1243" windowHeight="652" tabRatio="500" activeSheetId="2"/>
-    <customWorkbookView name="Jan Strube - Personal View" guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" mergeInterval="0" personalView="1" xWindow="-2" yWindow="54" windowWidth="1436" windowHeight="815" tabRatio="500" activeSheetId="5"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="238">
   <si>
     <t>Leader</t>
   </si>
@@ -779,6 +779,9 @@
   </si>
   <si>
     <t>SOI_YasuoArai_KEK_20140407.docx</t>
+  </si>
+  <si>
+    <t>AHCAL_FelixSefkow_DESY_20140410.docx</t>
   </si>
 </sst>
 </file>
@@ -965,14 +968,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1012,7 +1015,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{066A7CFC-D902-EF45-A5A7-3B6CF4E44A6D}" diskRevisions="1" revisionId="134" version="8">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{71122420-D25E-0840-8EB5-EDCD8CABF1E4}" diskRevisions="1" revisionId="136" version="9">
   <header guid="{90EFB229-A129-4641-96FB-C4C9036C70D7}" dateTime="2014-03-18T10:37:43" maxSheetId="6" userName="Jan Strube" r:id="rId1">
     <sheetIdMap count="5">
       <sheetId val="1"/>
@@ -1279,6 +1282,17 @@
       <sheetId val="7"/>
     </sheetIdMap>
   </header>
+  <header guid="{71122420-D25E-0840-8EB5-EDCD8CABF1E4}" dateTime="2014-04-10T10:06:10" maxSheetId="8" userName="Jan Strube" r:id="rId28" minRId="135" maxRId="136">
+    <sheetIdMap count="7">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -2596,6 +2610,29 @@
     <nc r="H9" t="inlineStr">
       <is>
         <t>SOI_YasuoArai_KEK_20140407.docx</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog28.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="135" sId="5" odxf="1" dxf="1" numFmtId="21">
+    <nc r="G9">
+      <v>41739</v>
+    </nc>
+    <odxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </odxf>
+    <ndxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="136" sId="5">
+    <nc r="H9" t="inlineStr">
+      <is>
+        <t>AHCAL_FelixSefkow_DESY_20140410.docx</t>
       </is>
     </nc>
   </rcc>
@@ -3375,10 +3412,10 @@
       <c r="B1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="37"/>
+      <c r="D1" s="39"/>
       <c r="E1" s="13" t="s">
         <v>1</v>
       </c>
@@ -3393,7 +3430,7 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="37" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3"/>
@@ -3408,7 +3445,7 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="39"/>
+      <c r="A3" s="37"/>
       <c r="B3" s="3"/>
       <c r="C3" s="38"/>
       <c r="D3" s="2" t="s">
@@ -3419,7 +3456,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="39"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="3"/>
       <c r="C4" s="6" t="s">
         <v>7</v>
@@ -3438,10 +3475,10 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="37" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -3455,8 +3492,8 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="39"/>
-      <c r="B6" s="39"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="37"/>
       <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
@@ -3465,8 +3502,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="30">
-      <c r="A7" s="39"/>
-      <c r="B7" s="39"/>
+      <c r="A7" s="37"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="7" t="s">
         <v>20</v>
       </c>
@@ -3478,7 +3515,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="30">
-      <c r="A8" s="39"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
@@ -3493,7 +3530,7 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="37" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -3507,7 +3544,7 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="39"/>
+      <c r="A10" s="37"/>
       <c r="C10" s="38" t="s">
         <v>30</v>
       </c>
@@ -3519,7 +3556,7 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="39"/>
+      <c r="A11" s="37"/>
       <c r="C11" s="38"/>
       <c r="D11" t="s">
         <v>35</v>
@@ -3529,7 +3566,7 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="39"/>
+      <c r="A12" s="37"/>
       <c r="C12" s="6" t="s">
         <v>37</v>
       </c>
@@ -3541,7 +3578,7 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="37" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -3555,7 +3592,7 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="39"/>
+      <c r="A14" s="37"/>
       <c r="C14" s="6" t="s">
         <v>41</v>
       </c>
@@ -3567,7 +3604,7 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="39"/>
+      <c r="A15" s="37"/>
       <c r="C15" s="6" t="s">
         <v>29</v>
       </c>
@@ -3579,7 +3616,7 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="37" t="s">
         <v>44</v>
       </c>
       <c r="C16" t="s">
@@ -3593,7 +3630,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="30">
-      <c r="A17" s="39"/>
+      <c r="A17" s="37"/>
       <c r="C17" s="4" t="s">
         <v>48</v>
       </c>
@@ -3613,7 +3650,7 @@
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="37" t="s">
         <v>51</v>
       </c>
       <c r="C19" t="s">
@@ -3627,7 +3664,7 @@
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="39"/>
+      <c r="A20" s="37"/>
       <c r="C20" t="s">
         <v>45</v>
       </c>
@@ -3639,7 +3676,7 @@
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="37" t="s">
         <v>58</v>
       </c>
       <c r="C21" t="s">
@@ -3653,7 +3690,7 @@
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="39"/>
+      <c r="A22" s="37"/>
       <c r="B22" t="s">
         <v>65</v>
       </c>
@@ -3694,27 +3731,27 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" topLeftCell="B1">
+      <selection activeCell="H22" sqref="H22"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
       <selection activeCell="E24" sqref="E24"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" topLeftCell="B1">
-      <selection activeCell="H22" sqref="H22"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
   </customSheetViews>
   <mergeCells count="11">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A5:A8"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A19:A20"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A5:A8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
@@ -3752,8 +3789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3773,10 +3810,10 @@
       <c r="A1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="37"/>
+      <c r="C1" s="39"/>
       <c r="D1" s="13" t="s">
         <v>1</v>
       </c>
@@ -3786,10 +3823,10 @@
       <c r="F1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="37"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="34" t="s">
@@ -4081,12 +4118,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
+      <selection activeCell="H16" sqref="H16"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" topLeftCell="B1">
       <selection activeCell="F14" sqref="F14"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
-      <selection activeCell="H16" sqref="H16"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
@@ -4134,10 +4171,10 @@
       <c r="A1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="37"/>
+      <c r="C1" s="39"/>
       <c r="D1" s="13" t="s">
         <v>1</v>
       </c>
@@ -4147,10 +4184,10 @@
       <c r="F1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="37"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="41" t="s">
@@ -4195,11 +4232,11 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
+      <selection activeCell="G5" sqref="G5"/>
+    </customSheetView>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
       <selection activeCell="E3" sqref="E3"/>
-    </customSheetView>
-    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
-      <selection activeCell="G5" sqref="G5"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="7">
@@ -4481,12 +4518,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
       <selection activeCell="C7" sqref="C7"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
@@ -4524,8 +4561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4697,6 +4734,12 @@
       <c r="F9" t="s">
         <v>72</v>
       </c>
+      <c r="G9" s="15">
+        <v>41739</v>
+      </c>
+      <c r="H9" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="20" t="s">
@@ -4898,12 +4941,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
-      <selection activeCell="F8" sqref="F8"/>
-    </customSheetView>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
       <selection activeCell="G20" sqref="G20"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
+      <selection activeCell="F8" sqref="F8"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="5">
@@ -4948,8 +4991,8 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
   <customSheetViews>
+    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}"/>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}"/>
-    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}"/>
   </customSheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Adding contributions from the VIP pixel chips
git-svn-id: svn+ssh://svn.cern.ch/reps/jansvn/trunk/lcDetRnD@534 4525493e-7705-40b1-a816-d608a930855b
</commit_message>
<xml_diff>
--- a/ListOfGroups.xlsx
+++ b/ListOfGroups.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="0" windowWidth="28720" windowHeight="17380" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="-40" yWindow="0" windowWidth="28720" windowHeight="17380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TPC" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,8 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="TITOV Maksym - Personal View" guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1243" windowHeight="652" tabRatio="500" activeSheetId="2"/>
     <customWorkbookView name="Jan Strube - Personal View" guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" mergeInterval="0" personalView="1" xWindow="-2" yWindow="54" windowWidth="1436" windowHeight="815" tabRatio="500" activeSheetId="5"/>
-    <customWorkbookView name="TITOV Maksym - Personal View" guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1243" windowHeight="652" tabRatio="500" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="239">
   <si>
     <t>Leader</t>
   </si>
@@ -782,6 +782,9 @@
   </si>
   <si>
     <t>AHCAL_FelixSefkow_DESY_20140410.docx</t>
+  </si>
+  <si>
+    <t>3DPixel_RonLipton_FNAL_20140410.docx</t>
   </si>
 </sst>
 </file>
@@ -968,14 +971,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1015,7 +1018,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{71122420-D25E-0840-8EB5-EDCD8CABF1E4}" diskRevisions="1" revisionId="136" version="9">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{6BCB8514-64F9-584F-929A-31E5D59EA1D8}" diskRevisions="1" revisionId="138" version="10">
   <header guid="{90EFB229-A129-4641-96FB-C4C9036C70D7}" dateTime="2014-03-18T10:37:43" maxSheetId="6" userName="Jan Strube" r:id="rId1">
     <sheetIdMap count="5">
       <sheetId val="1"/>
@@ -1293,6 +1296,17 @@
       <sheetId val="7"/>
     </sheetIdMap>
   </header>
+  <header guid="{6BCB8514-64F9-584F-929A-31E5D59EA1D8}" dateTime="2014-04-10T22:52:05" maxSheetId="8" userName="Jan Strube" r:id="rId29" minRId="137" maxRId="138">
+    <sheetIdMap count="7">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -2635,6 +2649,26 @@
         <t>AHCAL_FelixSefkow_DESY_20140410.docx</t>
       </is>
     </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog29.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="137" sId="2" numFmtId="19">
+    <nc r="G6">
+      <v>41739</v>
+    </nc>
+  </rcc>
+  <rcc rId="138" sId="2" xfDxf="1" dxf="1">
+    <nc r="H6" t="inlineStr">
+      <is>
+        <t>3DPixel_RonLipton_FNAL_20140410.docx</t>
+      </is>
+    </nc>
+    <ndxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </ndxf>
   </rcc>
 </revisions>
 </file>
@@ -3412,10 +3446,10 @@
       <c r="B1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="39"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="13" t="s">
         <v>1</v>
       </c>
@@ -3430,7 +3464,7 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3"/>
@@ -3445,7 +3479,7 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="37"/>
+      <c r="A3" s="39"/>
       <c r="B3" s="3"/>
       <c r="C3" s="38"/>
       <c r="D3" s="2" t="s">
@@ -3456,7 +3490,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="37"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="3"/>
       <c r="C4" s="6" t="s">
         <v>7</v>
@@ -3475,10 +3509,10 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="39" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -3492,8 +3526,8 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="37"/>
-      <c r="B6" s="37"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="39"/>
       <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
@@ -3502,8 +3536,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="30">
-      <c r="A7" s="37"/>
-      <c r="B7" s="37"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="39"/>
       <c r="C7" s="7" t="s">
         <v>20</v>
       </c>
@@ -3515,7 +3549,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="30">
-      <c r="A8" s="37"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
@@ -3530,7 +3564,7 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="39" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -3544,7 +3578,7 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="37"/>
+      <c r="A10" s="39"/>
       <c r="C10" s="38" t="s">
         <v>30</v>
       </c>
@@ -3556,7 +3590,7 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="37"/>
+      <c r="A11" s="39"/>
       <c r="C11" s="38"/>
       <c r="D11" t="s">
         <v>35</v>
@@ -3566,7 +3600,7 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="37"/>
+      <c r="A12" s="39"/>
       <c r="C12" s="6" t="s">
         <v>37</v>
       </c>
@@ -3578,7 +3612,7 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="39" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -3592,7 +3626,7 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="37"/>
+      <c r="A14" s="39"/>
       <c r="C14" s="6" t="s">
         <v>41</v>
       </c>
@@ -3604,7 +3638,7 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="37"/>
+      <c r="A15" s="39"/>
       <c r="C15" s="6" t="s">
         <v>29</v>
       </c>
@@ -3616,7 +3650,7 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="39" t="s">
         <v>44</v>
       </c>
       <c r="C16" t="s">
@@ -3630,7 +3664,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="30">
-      <c r="A17" s="37"/>
+      <c r="A17" s="39"/>
       <c r="C17" s="4" t="s">
         <v>48</v>
       </c>
@@ -3650,7 +3684,7 @@
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="39" t="s">
         <v>51</v>
       </c>
       <c r="C19" t="s">
@@ -3664,7 +3698,7 @@
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="37"/>
+      <c r="A20" s="39"/>
       <c r="C20" t="s">
         <v>45</v>
       </c>
@@ -3676,7 +3710,7 @@
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="39" t="s">
         <v>58</v>
       </c>
       <c r="C21" t="s">
@@ -3690,7 +3724,7 @@
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="37"/>
+      <c r="A22" s="39"/>
       <c r="B22" t="s">
         <v>65</v>
       </c>
@@ -3731,27 +3765,27 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
+      <selection activeCell="E24" sqref="E24"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" topLeftCell="B1">
       <selection activeCell="H22" sqref="H22"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
-      <selection activeCell="E24" sqref="E24"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
   </customSheetViews>
   <mergeCells count="11">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A5:A8"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A19:A20"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A5:A8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
@@ -3789,8 +3823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3810,10 +3844,10 @@
       <c r="A1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="39"/>
+      <c r="C1" s="37"/>
       <c r="D1" s="13" t="s">
         <v>1</v>
       </c>
@@ -3823,10 +3857,10 @@
       <c r="F1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="39"/>
+      <c r="H1" s="37"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="34" t="s">
@@ -3926,6 +3960,12 @@
       </c>
       <c r="F6" s="8" t="s">
         <v>78</v>
+      </c>
+      <c r="G6" s="35">
+        <v>41739</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -4118,12 +4158,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" topLeftCell="B1">
+      <selection activeCell="F14" sqref="F14"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
       <selection activeCell="H16" sqref="H16"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" topLeftCell="B1">
-      <selection activeCell="F14" sqref="F14"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
@@ -4171,10 +4211,10 @@
       <c r="A1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="39"/>
+      <c r="C1" s="37"/>
       <c r="D1" s="13" t="s">
         <v>1</v>
       </c>
@@ -4184,10 +4224,10 @@
       <c r="F1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="39"/>
+      <c r="H1" s="37"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="41" t="s">
@@ -4232,11 +4272,11 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
+      <selection activeCell="E3" sqref="E3"/>
+    </customSheetView>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
       <selection activeCell="G5" sqref="G5"/>
-    </customSheetView>
-    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
-      <selection activeCell="E3" sqref="E3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="7">
@@ -4518,12 +4558,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
+      <selection activeCell="C7" sqref="C7"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
       <selection activeCell="A6" sqref="A6:XFD6"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
-      <selection activeCell="C7" sqref="C7"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
@@ -4561,8 +4601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4941,12 +4981,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
+      <selection activeCell="F8" sqref="F8"/>
+    </customSheetView>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
       <selection activeCell="G20" sqref="G20"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
-      <selection activeCell="F8" sqref="F8"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="5">
@@ -4991,8 +5031,8 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
   <customSheetViews>
+    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}"/>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}"/>
-    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}"/>
   </customSheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Adding source from Frank Simon. Updates to the Excel spreadsheet
git-svn-id: svn+ssh://svn.cern.ch/reps/jansvn/trunk/lcDetRnD@552 4525493e-7705-40b1-a816-d608a930855b
</commit_message>
<xml_diff>
--- a/ListOfGroups.xlsx
+++ b/ListOfGroups.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="0" windowWidth="28720" windowHeight="17380" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="-40" yWindow="0" windowWidth="28720" windowHeight="17380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TPC" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,8 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jan Strube - Personal View" guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" mergeInterval="0" personalView="1" xWindow="-2" yWindow="54" windowWidth="1436" windowHeight="815" tabRatio="500" activeSheetId="5"/>
     <customWorkbookView name="TITOV Maksym - Personal View" guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1243" windowHeight="652" tabRatio="500" activeSheetId="2"/>
-    <customWorkbookView name="Jan Strube - Personal View" guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" mergeInterval="0" personalView="1" xWindow="-2" yWindow="54" windowWidth="1436" windowHeight="815" tabRatio="500" activeSheetId="5"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="246">
   <si>
     <t>Leader</t>
   </si>
@@ -796,6 +796,15 @@
   </si>
   <si>
     <t>Calorimeter_SiliconTungstenILD_VincentBoudry_IN2P3_20140323.docx</t>
+  </si>
+  <si>
+    <t>Calorimeter_SiliconTungstenILD_KiyotomeKawagoe_Kyushu_20140501.pdf</t>
+  </si>
+  <si>
+    <t>email, incomplete</t>
+  </si>
+  <si>
+    <t>Calorimeter_CLICdp_FrankSimon_MPI_20140506.pdf</t>
   </si>
 </sst>
 </file>
@@ -981,14 +990,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1028,273 +1037,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{5A5B8656-D36E-DD4B-A30D-CD5013FAD849}" diskRevisions="1" revisionId="146" version="12">
-  <header guid="{90EFB229-A129-4641-96FB-C4C9036C70D7}" dateTime="2014-03-18T10:37:43" maxSheetId="6" userName="Jan Strube" r:id="rId1">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{8C629D3D-FF3D-5D44-8037-C1BB23779435}" dateTime="2014-03-18T22:19:39" maxSheetId="6" userName="Jan Strube" r:id="rId2" minRId="1" maxRId="11">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{9482A396-4AA1-455D-9254-3A2438979D27}" dateTime="2014-03-19T11:40:52" maxSheetId="6" userName="TITOV Maksym" r:id="rId3" minRId="12" maxRId="13">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{4003C925-A84F-4F9F-B756-7920D044B967}" dateTime="2014-03-19T11:51:40" maxSheetId="6" userName="TITOV Maksym" r:id="rId4" minRId="14" maxRId="15">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{C61E7606-1614-4375-9F5F-47C3F5E1496B}" dateTime="2014-03-19T12:02:23" maxSheetId="6" userName="TITOV Maksym" r:id="rId5" minRId="16" maxRId="21">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{36F1A11B-2ECF-483C-944D-A55CC84FE9A4}" dateTime="2014-03-19T12:03:39" maxSheetId="6" userName="TITOV Maksym" r:id="rId6" minRId="22" maxRId="23">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{8F7BA7B1-BCBF-4D43-8B3F-49433647E38A}" dateTime="2014-03-19T12:04:04" maxSheetId="6" userName="TITOV Maksym" r:id="rId7" minRId="24" maxRId="25">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{5E25232B-25B5-4D1B-A1D2-7F3DC8A68A77}" dateTime="2014-03-19T17:58:43" maxSheetId="6" userName="TITOV Maksym" r:id="rId8" minRId="26" maxRId="34">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{1BC67F2F-6052-4633-BA03-7212EB151D3A}" dateTime="2014-03-19T18:01:19" maxSheetId="6" userName="TITOV Maksym" r:id="rId9" minRId="35" maxRId="43">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{877E2EB7-19C2-4EBC-8170-4A1C55C74FE9}" dateTime="2014-03-19T18:04:36" maxSheetId="6" userName="TITOV Maksym" r:id="rId10" minRId="44">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{43271ECA-8F72-49B1-8E24-5C904F2DA8F2}" dateTime="2014-03-19T18:07:08" maxSheetId="6" userName="TITOV Maksym" r:id="rId11" minRId="45" maxRId="52">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{76BD215A-123E-4672-9073-F1C110958708}" dateTime="2014-03-19T18:11:06" maxSheetId="6" userName="TITOV Maksym" r:id="rId12" minRId="53">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{6D9D7D41-50C8-464D-9BF7-5BC4F5612D9F}" dateTime="2014-03-20T07:52:14" maxSheetId="6" userName="TITOV Maksym" r:id="rId13" minRId="54">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{979D76EA-7A67-43DE-ABAF-828B34B07042}" dateTime="2014-03-20T07:55:52" maxSheetId="6" userName="TITOV Maksym" r:id="rId14" minRId="55" maxRId="59">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{2A707E59-1FD4-439E-A3FA-C017AAA5AA92}" dateTime="2014-03-20T07:57:21" maxSheetId="6" userName="TITOV Maksym" r:id="rId15" minRId="60" maxRId="61">
-    <sheetIdMap count="5">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{C64DB0C3-AC9E-405C-8E5F-D601774AA2DA}" dateTime="2014-03-20T08:03:52" maxSheetId="7" userName="TITOV Maksym" r:id="rId16" minRId="62" maxRId="67">
-    <sheetIdMap count="6">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-      <sheetId val="6"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{F1622155-C3DA-1C4B-ABDA-A0CE26E9D8E3}" dateTime="2014-03-21T01:56:45" maxSheetId="8" userName="Jan Strube" r:id="rId17" minRId="68" maxRId="78">
-    <sheetIdMap count="7">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-      <sheetId val="6"/>
-      <sheetId val="7"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{77DFF067-4434-804C-A748-4AF665DF414F}" dateTime="2014-03-23T01:42:17" maxSheetId="8" userName="Jan Strube" r:id="rId18" minRId="79" maxRId="85">
-    <sheetIdMap count="7">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-      <sheetId val="6"/>
-      <sheetId val="7"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{9A6BF651-ABE4-E541-B536-3AEFBC556923}" dateTime="2014-03-23T01:43:50" maxSheetId="8" userName="Jan Strube" r:id="rId19">
-    <sheetIdMap count="7">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-      <sheetId val="6"/>
-      <sheetId val="7"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{6E767D04-EB2B-744A-BE3E-38D5BBE714DB}" dateTime="2014-03-23T02:30:44" maxSheetId="8" userName="Jan Strube" r:id="rId20" minRId="86" maxRId="92">
-    <sheetIdMap count="7">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-      <sheetId val="6"/>
-      <sheetId val="7"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{AD5617E4-C62E-0746-A7C9-5D96D7D4DE27}" dateTime="2014-03-23T02:32:14" maxSheetId="8" userName="Jan Strube" r:id="rId21">
-    <sheetIdMap count="7">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-      <sheetId val="6"/>
-      <sheetId val="7"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{DB2702CC-435E-D146-B4C9-AE60ADA8C4EB}" dateTime="2014-03-25T17:00:47" maxSheetId="8" userName="Jan Strube" r:id="rId22" minRId="93" maxRId="106">
-    <sheetIdMap count="7">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-      <sheetId val="6"/>
-      <sheetId val="7"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{FAE6AD53-8B02-964B-9E03-2DA6A505E01F}" dateTime="2014-04-05T13:14:05" maxSheetId="8" userName="Jan Strube" r:id="rId23" minRId="107" maxRId="113">
-    <sheetIdMap count="7">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-      <sheetId val="6"/>
-      <sheetId val="7"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{4101B9EF-F6AE-5D4D-9600-DC73FEFB3B43}" dateTime="2014-04-05T13:50:08" maxSheetId="8" userName="Jan Strube" r:id="rId24" minRId="114" maxRId="128">
-    <sheetIdMap count="7">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-      <sheetId val="6"/>
-      <sheetId val="7"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{97119F5E-1AE8-DD4E-A39E-4B9FDBC962E5}" dateTime="2014-04-06T23:07:02" maxSheetId="8" userName="Jan Strube" r:id="rId25" minRId="129" maxRId="131">
-    <sheetIdMap count="7">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-      <sheetId val="6"/>
-      <sheetId val="7"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{E10FDDBA-7369-7F46-9E10-0216F9A48312}" dateTime="2014-04-06T23:07:54" maxSheetId="8" userName="Jan Strube" r:id="rId26" minRId="132">
-    <sheetIdMap count="7">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-      <sheetId val="6"/>
-      <sheetId val="7"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{066A7CFC-D902-EF45-A5A7-3B6CF4E44A6D}" dateTime="2014-04-07T17:48:14" maxSheetId="8" userName="Jan Strube" r:id="rId27" minRId="133" maxRId="134">
-    <sheetIdMap count="7">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-      <sheetId val="6"/>
-      <sheetId val="7"/>
-    </sheetIdMap>
-  </header>
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{AC3FBE52-88DD-8E4A-B5FB-5664F571FB55}" diskRevisions="1" revisionId="154" version="13">
   <header guid="{71122420-D25E-0840-8EB5-EDCD8CABF1E4}" dateTime="2014-04-10T10:06:10" maxSheetId="8" userName="Jan Strube" r:id="rId28" minRId="135" maxRId="136">
     <sheetIdMap count="7">
       <sheetId val="1"/>
@@ -1339,488 +1082,25 @@
       <sheetId val="7"/>
     </sheetIdMap>
   </header>
+  <header guid="{AC3FBE52-88DD-8E4A-B5FB-5664F571FB55}" dateTime="2014-05-08T14:03:30" maxSheetId="8" userName="Jan Strube" r:id="rId32" minRId="147" maxRId="154">
+    <sheetIdMap count="7">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
 <file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
-</file>
-
-<file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="44" sId="5">
-    <nc r="A23" t="inlineStr">
-      <is>
-        <t>SLAC</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="45" sId="5">
-    <oc r="A23" t="inlineStr">
-      <is>
-        <t>SLAC</t>
-      </is>
-    </oc>
-    <nc r="A23" t="inlineStr">
-      <is>
-        <t>KPIX</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="46" sId="5">
-    <nc r="B23" t="inlineStr">
-      <is>
-        <t>SLAC</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="47" sId="5">
-    <nc r="C23" t="inlineStr">
-      <is>
-        <t>Marty Breidenbach</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="48" sId="5">
-    <nc r="D23" t="inlineStr">
-      <is>
-        <t>mib@slac.stanford.edu</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="49" sId="5" odxf="1" dxf="1" numFmtId="19">
-    <nc r="E23">
-      <v>41711</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="50" sId="5">
-    <nc r="F23" t="inlineStr">
-      <is>
-        <t>Jan</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="51" sId="5" odxf="1" dxf="1" numFmtId="19">
-    <nc r="G23">
-      <v>41716</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="52" sId="5">
-    <nc r="H23" t="inlineStr">
-      <is>
-        <t>KPiX_RD_Status.docx</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="53" sId="5">
-    <oc r="A16" t="inlineStr">
-      <is>
-        <t>Si ECAL</t>
-      </is>
-    </oc>
-    <nc r="A16" t="inlineStr">
-      <is>
-        <t>Si-W ECAL</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog13.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="54" sId="3" numFmtId="21">
-    <oc r="E3">
-      <v>41705</v>
-    </oc>
-    <nc r="E3">
-      <v>41718</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog14.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rfmt sheetId="2" sqref="B11" start="0" length="0">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="C11" start="0" length="0">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="D11" start="0" length="0">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="E11" start="0" length="0">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" s="1" sqref="F11" start="0" length="0">
-    <dxf>
-      <font>
-        <u/>
-        <sz val="12"/>
-        <color theme="10"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="G11" start="0" length="0">
-    <dxf>
-      <numFmt numFmtId="21" formatCode="dd\-mmm"/>
-      <alignment horizontal="general" vertical="bottom" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="H11" start="0" length="0">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="55" sId="2">
-    <nc r="C11" t="inlineStr">
-      <is>
-        <t>Bruce Schumm</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="C11">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="56" sId="2">
-    <nc r="B11" t="inlineStr">
-      <is>
-        <t>SCIPP, UCSC</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="B11">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="57" sId="2">
-    <nc r="D11" t="inlineStr">
-      <is>
-        <t>schumm@scipp.ucsc.edu</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="58" sId="2" odxf="1" dxf="1" numFmtId="19">
-    <nc r="E11">
-      <v>41711</v>
-    </nc>
-    <ndxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="59" sId="2">
-    <nc r="F11" t="inlineStr">
-      <is>
-        <t>Jan</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog15.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="60" sId="5" odxf="1" dxf="1" numFmtId="19">
-    <nc r="E8">
-      <v>41711</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="61" sId="5">
-    <nc r="F8" t="inlineStr">
-      <is>
-        <t>Jan</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog16.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <ris rId="62" sheetId="6" name="[ListOfGroups_20032014.xlsx]Sheet1" sheetPosition="5"/>
-  <rcc rId="63" sId="2">
-    <nc r="B14" t="inlineStr">
-      <is>
-        <t>CERN</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="64" sId="2">
-    <nc r="C14" t="inlineStr">
-      <is>
-        <t>Lucie Linsen</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="65" sId="2">
-    <nc r="D14" t="inlineStr">
-      <is>
-        <t>lucie.linsen@cern.ch</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="66" sId="2" numFmtId="19">
-    <nc r="E14">
-      <v>41718</v>
-    </nc>
-  </rcc>
-  <rcc rId="67" sId="2">
-    <nc r="F14" t="inlineStr">
-      <is>
-        <t>Maxim</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcv guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" action="delete"/>
-  <rcv guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog17.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <ris rId="68" sheetId="7" name="[ListOfGroups_20032014.xlsx]Sheet2" sheetPosition="6"/>
-  <rrc rId="69" sId="4" ref="A8:XFD8" action="deleteRow">
-    <rfmt sheetId="4" xfDxf="1" sqref="A8:XFD8" start="0" length="0"/>
-    <rcc rId="0" sId="4" dxf="1">
-      <nc r="A8" t="inlineStr">
-        <is>
-          <t>GEM calorimetry</t>
-        </is>
-      </nc>
-      <ndxf>
-        <alignment horizontal="center" vertical="center" readingOrder="0"/>
-      </ndxf>
-    </rcc>
-    <rfmt sheetId="4" sqref="B8" start="0" length="0">
-      <dxf>
-        <alignment horizontal="center" vertical="center" readingOrder="0"/>
-      </dxf>
-    </rfmt>
-    <rcc rId="0" sId="4" dxf="1">
-      <nc r="C8" t="inlineStr">
-        <is>
-          <t>UT Arlington</t>
-        </is>
-      </nc>
-      <ndxf>
-        <alignment horizontal="center" vertical="center" readingOrder="0"/>
-      </ndxf>
-    </rcc>
-    <rcc rId="0" sId="4">
-      <nc r="D8" t="inlineStr">
-        <is>
-          <t>Andy White</t>
-        </is>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="4" s="1" dxf="1">
-      <nc r="E8" t="inlineStr">
-        <is>
-          <t>awhite@uta.edu</t>
-        </is>
-      </nc>
-      <ndxf>
-        <font>
-          <u/>
-          <sz val="12"/>
-          <color theme="10"/>
-          <name val="Calibri"/>
-          <scheme val="minor"/>
-        </font>
-      </ndxf>
-    </rcc>
-  </rrc>
-  <rrc rId="70" sId="4" ref="A8:XFD8" action="deleteRow">
-    <rfmt sheetId="4" xfDxf="1" sqref="A8:XFD8" start="0" length="0"/>
-    <rfmt sheetId="4" sqref="A8" start="0" length="0">
-      <dxf>
-        <alignment horizontal="center" vertical="center" readingOrder="0"/>
-      </dxf>
-    </rfmt>
-    <rfmt sheetId="4" sqref="B8" start="0" length="0">
-      <dxf>
-        <alignment horizontal="center" vertical="center" readingOrder="0"/>
-      </dxf>
-    </rfmt>
-    <rfmt sheetId="4" sqref="C8" start="0" length="0">
-      <dxf>
-        <alignment horizontal="center" vertical="center" readingOrder="0"/>
-      </dxf>
-    </rfmt>
-    <rcc rId="0" sId="4">
-      <nc r="D8" t="inlineStr">
-        <is>
-          <t>Jae Yu</t>
-        </is>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="4" s="1" dxf="1">
-      <nc r="E8" t="inlineStr">
-        <is>
-          <t>jaehoonyu@uta.edu</t>
-        </is>
-      </nc>
-      <ndxf>
-        <font>
-          <u/>
-          <sz val="12"/>
-          <color theme="10"/>
-          <name val="Calibri"/>
-          <scheme val="minor"/>
-        </font>
-      </ndxf>
-    </rcc>
-  </rrc>
-  <rfmt sheetId="1" sqref="A24" start="0" length="0">
-    <dxf>
-      <font>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="71" sId="1" odxf="1" dxf="1">
-    <nc r="B24" t="inlineStr">
-      <is>
-        <t>Bonn</t>
-      </is>
-    </nc>
-    <odxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </odxf>
-    <ndxf>
-      <alignment horizontal="right" readingOrder="0"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="72" sId="1" odxf="1" dxf="1">
-    <nc r="C24" t="inlineStr">
-      <is>
-        <t>Jochen Kaminski</t>
-      </is>
-    </nc>
-    <odxf>
-      <alignment horizontal="right" readingOrder="0"/>
-    </odxf>
-    <ndxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="73" sId="1" odxf="1" s="1" dxf="1">
-    <nc r="D24" t="inlineStr">
-      <is>
-        <t>kaminski@physik.uni-bonn.de</t>
-      </is>
-    </nc>
-    <odxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </odxf>
-    <ndxf>
-      <font>
-        <u/>
-        <sz val="12"/>
-        <color theme="10"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </ndxf>
-  </rcc>
-  <rcc rId="74" sId="1" odxf="1" dxf="1" numFmtId="21">
-    <nc r="E24">
-      <v>41710</v>
+  <rcc rId="147" sId="5" odxf="1" dxf="1" numFmtId="21">
+    <nc r="G5">
+      <v>41761</v>
     </nc>
     <odxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1829,56 +1109,31 @@
       <numFmt numFmtId="21" formatCode="d\-mmm"/>
     </ndxf>
   </rcc>
-  <rcc rId="75" sId="1" odxf="1">
-    <nc r="F24" t="inlineStr">
+  <rfmt sheetId="5" xfDxf="1" sqref="H5" start="0" length="0"/>
+  <rcc rId="148" sId="5">
+    <nc r="H5" t="inlineStr">
+      <is>
+        <t>Calorimeter_SiliconTungstenILD_KiyotomeKawagoe_Kyushu_20140501.pdf</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="149" sId="5">
+    <nc r="H7" t="inlineStr">
+      <is>
+        <t>email, incomplete</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="150" sId="1">
+    <nc r="G3" t="inlineStr">
       <is>
         <t>Maxim</t>
       </is>
     </nc>
-    <odxf/>
   </rcc>
-  <rcc rId="76" sId="1" odxf="1" dxf="1" numFmtId="21">
-    <nc r="G24">
-      <v>41712</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="top" readingOrder="0"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
-      <alignment horizontal="general" vertical="bottom" readingOrder="0"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="77" sId="1" odxf="1" dxf="1">
-    <nc r="H24" t="inlineStr">
-      <is>
-        <t>Input_LC_detector_RnD_liaison_report_from_Bonn.pdf</t>
-      </is>
-    </nc>
-    <odxf>
-      <alignment horizontal="center" vertical="top" readingOrder="0"/>
-    </odxf>
-    <ndxf>
-      <alignment horizontal="general" vertical="bottom" readingOrder="0"/>
-    </ndxf>
-  </rcc>
-  <rfmt sheetId="1" sqref="A24:XFD24" start="0" length="0">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rm rId="78" sheetId="1" source="B24:I24" destination="C24:J24" sourceSheetId="1"/>
-  <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="delete"/>
-  <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog18.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="79" sId="5" odxf="1" dxf="1" numFmtId="21">
-    <nc r="E5">
-      <v>41718</v>
+  <rcc rId="151" sId="1" odxf="1" dxf="1" numFmtId="21">
+    <nc r="F3">
+      <v>41754</v>
     </nc>
     <odxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1887,775 +1142,16 @@
       <numFmt numFmtId="21" formatCode="d\-mmm"/>
     </ndxf>
   </rcc>
-  <rcc rId="80" sId="5">
-    <nc r="F5" t="inlineStr">
-      <is>
-        <t>Jan</t>
-      </is>
+  <rrc rId="152" sId="5" ref="A20:XFD20" action="insertRow"/>
+  <rcc rId="153" sId="5" numFmtId="21">
+    <nc r="G20">
+      <v>41765</v>
     </nc>
   </rcc>
-  <rcc rId="81" sId="5" odxf="1" dxf="1">
-    <nc r="A18" t="inlineStr">
+  <rcc rId="154" sId="5" xfDxf="1" dxf="1">
+    <nc r="H20" t="inlineStr">
       <is>
-        <t>CLIC</t>
-      </is>
-    </nc>
-    <odxf>
-      <font>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="bottom" readingOrder="0"/>
-    </odxf>
-    <ndxf>
-      <font>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Courier"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="center" readingOrder="0"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="82" sId="5">
-    <nc r="B18" t="inlineStr">
-      <is>
-        <t>MPI</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="83" sId="5">
-    <nc r="C18" t="inlineStr">
-      <is>
-        <t>Frank Simon</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="84" sId="5">
-    <nc r="D18" t="inlineStr">
-      <is>
-        <t>frank.simon@cern.ch</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="85" sId="5" odxf="1" dxf="1" numFmtId="19">
-    <nc r="E18">
-      <v>41718</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
-    </ndxf>
-  </rcc>
-  <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="delete"/>
-  <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog19.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="delete"/>
-  <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="1" sId="4">
-    <nc r="G1" t="inlineStr">
-      <is>
-        <t>by</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="2" sId="4" odxf="1" dxf="1">
-    <nc r="F1" t="inlineStr">
-      <is>
-        <t>contacted on</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </ndxf>
-  </rcc>
-  <rfmt sheetId="4" sqref="G1" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="3" sId="4">
-    <nc r="G3" t="inlineStr">
-      <is>
-        <t>Jan</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="4" sId="4" odxf="1" dxf="1" numFmtId="21">
-    <nc r="F3">
-      <v>41711</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="5" sId="4" odxf="1" dxf="1" numFmtId="21">
-    <nc r="F7">
-      <v>41711</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="6" sId="4">
-    <nc r="G7" t="inlineStr">
-      <is>
-        <t>Jan</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="7" sId="4" odxf="1" dxf="1" numFmtId="21">
-    <nc r="F17">
-      <v>41711</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="8" sId="4">
-    <nc r="G17" t="inlineStr">
-      <is>
-        <t>Jan</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="9" sId="4">
-    <nc r="H1" t="inlineStr">
-      <is>
-        <t>response received</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="4" sqref="H1" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="10" sId="4" odxf="1" dxf="1" numFmtId="21">
-    <nc r="H17">
-      <v>41716</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="11" sId="4">
-    <nc r="I17" t="inlineStr">
-      <is>
-        <t>KPiX_RD_Status.docx</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="delete"/>
-  <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog20.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rrc rId="86" sId="2" eol="1" ref="A15:XFD15" action="insertRow"/>
-  <rcc rId="87" sId="2">
-    <nc r="A15" t="inlineStr">
-      <is>
-        <t>Spanish Network</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="88" sId="2">
-    <nc r="B15" t="inlineStr">
-      <is>
-        <t>IFCA</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="89" sId="2">
-    <nc r="C15" t="inlineStr">
-      <is>
-        <t>Alberto Ruiz Jimeno</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="90" sId="2" xfDxf="1" dxf="1">
-    <nc r="D15" t="inlineStr">
-      <is>
-        <t>ruiz@ifca.unican.es</t>
-      </is>
-    </nc>
-    <ndxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="91" sId="2">
-    <nc r="F15" t="inlineStr">
-      <is>
-        <t>Jan</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="92" sId="2" numFmtId="19">
-    <nc r="E15">
-      <v>41721</v>
-    </nc>
-  </rcc>
-  <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="delete"/>
-  <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog21.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="delete"/>
-  <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog22.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="93" sId="2">
-    <nc r="A14" t="inlineStr">
-      <is>
-        <t>CLIC</t>
-      </is>
-    </nc>
-  </rcc>
-  <rrc rId="94" sId="2" ref="A15:XFD15" action="insertRow"/>
-  <rcc rId="95" sId="2">
-    <nc r="C15" t="inlineStr">
-      <is>
-        <t>Dominik Dannheim</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="96" sId="2">
-    <nc r="D15" t="inlineStr">
-      <is>
-        <t>dominik.dannheim@cern.ch</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="97" sId="2" numFmtId="19">
-    <nc r="E15">
-      <v>41723</v>
-    </nc>
-  </rcc>
-  <rcc rId="98" sId="2">
-    <nc r="F15" t="inlineStr">
-      <is>
-        <t>Jan</t>
-      </is>
-    </nc>
-  </rcc>
-  <rrc rId="99" sId="2" ref="A9:XFD9" action="insertRow"/>
-  <rcc rId="100" sId="2" numFmtId="19">
-    <nc r="E9">
-      <v>41723</v>
-    </nc>
-  </rcc>
-  <rrc rId="101" sId="5" ref="A13:XFD13" action="insertRow"/>
-  <rcc rId="102" sId="5" numFmtId="19">
-    <nc r="E13">
-      <v>41723</v>
-    </nc>
-  </rcc>
-  <rcc rId="103" sId="5" odxf="1" dxf="1" numFmtId="21">
-    <nc r="G7">
-      <v>41723</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="104" sId="5" odxf="1" dxf="1" numFmtId="21">
-    <nc r="E18">
-      <v>41723</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="105" sId="1" odxf="1" dxf="1" numFmtId="21">
-    <nc r="F4">
-      <v>41715</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="106" sId="1">
-    <nc r="G4" t="inlineStr">
-      <is>
-        <t>Jan</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog23.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="107" sId="2" odxf="1" dxf="1" numFmtId="21">
-    <nc r="G4">
-      <v>41732</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
-    </ndxf>
-  </rcc>
-  <rfmt sheetId="2" xfDxf="1" sqref="H4" start="0" length="0">
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="108" sId="2">
-    <nc r="H4" t="inlineStr">
-      <is>
-        <t>FPCCD_VTX_YasuhiroSugimoto_KEK_20140403.docx</t>
-      </is>
-    </nc>
-  </rcc>
-  <rm rId="109" sheetId="2" source="I10" destination="H10" sourceSheetId="2">
-    <rcc rId="0" sId="2" dxf="1">
-      <nc r="H10" t="inlineStr">
-        <is>
-          <t>Report received</t>
-        </is>
-      </nc>
-      <ndxf>
-        <numFmt numFmtId="21" formatCode="d\-mmm"/>
-      </ndxf>
-    </rcc>
-  </rm>
-  <rcc rId="110" sId="2" xfDxf="1" dxf="1">
-    <oc r="H10" t="inlineStr">
-      <is>
-        <t>KPiX_RD_Status.docx</t>
-      </is>
-    </oc>
-    <nc r="H10" t="inlineStr">
-      <is>
-        <t>Tracker_KPIX_MartyBreidenbach_SLAC_20140318.docx</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A1:A1048576">
-    <dxf>
-      <alignment vertical="center"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="A1:A1048576">
-    <dxf>
-      <alignment horizontal="left"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="A1:A1048576">
-    <dxf>
-      <alignment horizontal="general"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="A1:A1048576">
-    <dxf>
-      <alignment horizontal="left"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="A1:A1048576">
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="111" sId="2" odxf="1" dxf="1" numFmtId="21">
-    <nc r="G7">
-      <v>41734</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="112" sId="2" xfDxf="1" dxf="1">
-    <nc r="H7" t="inlineStr">
-      <is>
-        <t>Chronopixel_NickSinev_Oregon_20140405.docx</t>
-      </is>
-    </nc>
-    <ndxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="113" sId="2" xfDxf="1" dxf="1">
-    <nc r="H12" t="inlineStr">
-      <is>
-        <t>Tracker_SCIPPTracking_BruceSchumm_SCIPP_20140326.docx</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="G1:G1048576">
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="G1:G1048576">
-    <dxf>
-      <alignment horizontal="left"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="G1:G1048576">
-    <dxf>
-      <alignment horizontal="general"/>
-    </dxf>
-  </rfmt>
-  <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="delete"/>
-  <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog24.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="114" sId="2" numFmtId="19">
-    <nc r="G12">
-      <v>41724</v>
-    </nc>
-  </rcc>
-  <rcc rId="115" sId="2" xfDxf="1" dxf="1">
-    <nc r="H15" t="inlineStr">
-      <is>
-        <t>CLICPix_LucieLinssen_CERN_20140404.pdf</t>
-      </is>
-    </nc>
-    <ndxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="116" sId="2" numFmtId="19">
-    <nc r="G15">
-      <v>41733</v>
-    </nc>
-  </rcc>
-  <rrc rId="117" sId="2" ref="A4:XFD4" action="insertRow"/>
-  <rcc rId="118" sId="2">
-    <nc r="C4" t="inlineStr">
-      <is>
-        <t>Marcel Vos</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="119" sId="2">
-    <nc r="D4" t="inlineStr">
-      <is>
-        <t>marcel.vos@cern.ch</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="120" sId="2">
-    <nc r="C19" t="inlineStr">
-      <is>
-        <t>Marcel Vos</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="121" sId="2" odxf="1" s="1" dxf="1">
-    <nc r="D19" t="inlineStr">
-      <is>
-        <t>marcel.vos@cern.ch</t>
-      </is>
-    </nc>
-    <odxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </odxf>
-    <ndxf>
-      <font>
-        <u/>
-        <sz val="12"/>
-        <color theme="10"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </ndxf>
-  </rcc>
-  <rrc rId="122" sId="4" ref="A15:XFD15" action="deleteRow">
-    <rfmt sheetId="4" xfDxf="1" sqref="A15:XFD15" start="0" length="0"/>
-    <rcc rId="0" sId="4">
-      <nc r="A15" t="inlineStr">
-        <is>
-          <t>Kpix</t>
-        </is>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="4">
-      <nc r="C15" t="inlineStr">
-        <is>
-          <t>SLAC</t>
-        </is>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="4">
-      <nc r="D15" t="inlineStr">
-        <is>
-          <t>Marty Breidenbach</t>
-        </is>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="4" s="1" dxf="1">
-      <nc r="E15" t="inlineStr">
-        <is>
-          <t>mib@slac.stanford.edu</t>
-        </is>
-      </nc>
-      <ndxf>
-        <font>
-          <u/>
-          <sz val="12"/>
-          <color theme="10"/>
-          <name val="Calibri"/>
-          <scheme val="minor"/>
-        </font>
-      </ndxf>
-    </rcc>
-    <rcc rId="0" sId="4" dxf="1" numFmtId="21">
-      <nc r="F15">
-        <v>41711</v>
-      </nc>
-      <ndxf>
-        <numFmt numFmtId="21" formatCode="d\-mmm"/>
-      </ndxf>
-    </rcc>
-    <rcc rId="0" sId="4">
-      <nc r="G15" t="inlineStr">
-        <is>
-          <t>Jan</t>
-        </is>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="4" dxf="1" numFmtId="21">
-      <nc r="H15">
-        <v>41716</v>
-      </nc>
-      <ndxf>
-        <numFmt numFmtId="21" formatCode="d\-mmm"/>
-      </ndxf>
-    </rcc>
-    <rcc rId="0" sId="4">
-      <nc r="I15" t="inlineStr">
-        <is>
-          <t>KPiX_RD_Status.docx</t>
-        </is>
-      </nc>
-    </rcc>
-  </rrc>
-  <rrc rId="123" sId="4" ref="A3:XFD3" action="deleteRow">
-    <rfmt sheetId="4" xfDxf="1" sqref="A3:XFD3" start="0" length="0"/>
-    <rcc rId="0" sId="4">
-      <nc r="A3" t="inlineStr">
-        <is>
-          <t>Silicon Development</t>
-        </is>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="4">
-      <nc r="C3" t="inlineStr">
-        <is>
-          <t>SCIPP, UCSC</t>
-        </is>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="4">
-      <nc r="D3" t="inlineStr">
-        <is>
-          <t>Bruce Schumm</t>
-        </is>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="4" s="1" dxf="1">
-      <nc r="E3" t="inlineStr">
-        <is>
-          <t>schumm@scipp.ucsc.edu</t>
-        </is>
-      </nc>
-      <ndxf>
-        <font>
-          <u/>
-          <sz val="12"/>
-          <color theme="10"/>
-          <name val="Calibri"/>
-          <scheme val="minor"/>
-        </font>
-      </ndxf>
-    </rcc>
-    <rcc rId="0" sId="4" dxf="1" numFmtId="21">
-      <nc r="F3">
-        <v>41711</v>
-      </nc>
-      <ndxf>
-        <numFmt numFmtId="21" formatCode="d\-mmm"/>
-      </ndxf>
-    </rcc>
-    <rcc rId="0" sId="4">
-      <nc r="G3" t="inlineStr">
-        <is>
-          <t>Jan</t>
-        </is>
-      </nc>
-    </rcc>
-  </rrc>
-  <rfmt sheetId="3" sqref="G3" start="0" length="0">
-    <dxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="124" sId="3" xfDxf="1" dxf="1">
-    <nc r="H3" t="inlineStr">
-      <is>
-        <t>FCAL_WolfgangLohmann_DESY_20140327.pdf</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="125" sId="3" xfDxf="1" dxf="1">
-    <nc r="H4" t="inlineStr">
-      <is>
-        <t>FCAL_WolfgangLohmann_DESY_20140327.tar</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="126" sId="3" numFmtId="21">
-    <nc r="G3">
-      <v>41725</v>
-    </nc>
-  </rcc>
-  <rcc rId="127" sId="5">
-    <nc r="F19" t="inlineStr">
-      <is>
-        <t>Jan</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="128" sId="5" odxf="1" dxf="1" numFmtId="21">
-    <nc r="G19">
-      <v>41733</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
-    </ndxf>
-  </rcc>
-  <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="delete"/>
-  <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog25.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="129" sId="5" xfDxf="1" dxf="1">
-    <nc r="H19" t="inlineStr">
-      <is>
-        <t>CERN_LCDGroup_LucieLinssen_CERN_20140404.pdf</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="130" sId="5" xfDxf="1" dxf="1">
-    <nc r="H12" t="inlineStr">
-      <is>
-        <t>GEM_DHCAL_AndyWhite_UTA_20140326.doc</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="131" sId="5" odxf="1" dxf="1" numFmtId="21">
-    <nc r="G12">
-      <v>41724</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
-    </ndxf>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog26.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rm rId="132" sheetId="5" source="A15:D15" destination="A20:D20" sourceSheetId="5"/>
-  <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="delete"/>
-  <rcv guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog27.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="133" sId="2" numFmtId="19">
-    <nc r="G9">
-      <v>41736</v>
-    </nc>
-  </rcc>
-  <rcc rId="134" sId="2">
-    <nc r="H9" t="inlineStr">
-      <is>
-        <t>SOI_YasuoArai_KEK_20140407.docx</t>
+        <t>Calorimeter_CLICdp_FrankSimon_MPI_20140506.pdf</t>
       </is>
     </nc>
   </rcc>
@@ -2702,30 +1198,6 @@
       <alignment horizontal="center" readingOrder="0"/>
     </ndxf>
   </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="12" sId="5" odxf="1" dxf="1" numFmtId="19">
-    <nc r="E9">
-      <v>41717</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="13" sId="5">
-    <nc r="F9" t="inlineStr">
-      <is>
-        <t>Maxim</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcv guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" action="add"/>
 </revisions>
 </file>
 
@@ -2811,407 +1283,8 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="14" sId="5" odxf="1" dxf="1" numFmtId="19">
-    <nc r="E3">
-      <v>41717</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="15" sId="5">
-    <nc r="F3" t="inlineStr">
-      <is>
-        <t>Maxim</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="16" sId="5" odxf="1" dxf="1" numFmtId="19">
-    <nc r="E4">
-      <v>41717</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="17" sId="5">
-    <nc r="F4" t="inlineStr">
-      <is>
-        <t>Maxim</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="18" sId="5" odxf="1" dxf="1" numFmtId="19">
-    <nc r="E13">
-      <v>41717</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="19" sId="5">
-    <nc r="F13" t="inlineStr">
-      <is>
-        <t>Maxim</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="20" sId="5" odxf="1" dxf="1" numFmtId="19">
-    <nc r="E11">
-      <v>41717</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="21" sId="5">
-    <nc r="F11" t="inlineStr">
-      <is>
-        <t>Maxim</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="22" sId="5" odxf="1" dxf="1" numFmtId="19">
-    <nc r="E7">
-      <v>41711</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="23" sId="5">
-    <nc r="F7" t="inlineStr">
-      <is>
-        <t>Jan</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog7.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rfmt sheetId="5" sqref="E10" start="0" length="0">
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="24" sId="5">
-    <nc r="F10" t="inlineStr">
-      <is>
-        <t>Jan</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="25" sId="5" numFmtId="19">
-    <nc r="E10">
-      <v>41346</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog8.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="26" sId="5" odxf="1" dxf="1" numFmtId="19">
-    <nc r="E12">
-      <v>41711</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="27" sId="5">
-    <nc r="F12" t="inlineStr">
-      <is>
-        <t>Jan</t>
-      </is>
-    </nc>
-  </rcc>
-  <rrc rId="28" sId="5" eol="1" ref="A16:XFD16" action="insertRow"/>
-  <rcc rId="29" sId="5">
-    <nc r="A16" t="inlineStr">
-      <is>
-        <t>Si ECAL</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="5" sqref="A16">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Courier"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="30" sId="5">
-    <nc r="B16" t="inlineStr">
-      <is>
-        <t>U Oregon</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="31" sId="5">
-    <nc r="C16" t="inlineStr">
-      <is>
-        <t>David Strom</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="32" sId="5" odxf="1" s="1" dxf="1">
-    <nc r="D16" t="inlineStr">
-      <is>
-        <t>dstrom@uoregon.edu</t>
-      </is>
-    </nc>
-    <odxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </odxf>
-    <ndxf>
-      <font>
-        <u/>
-        <sz val="12"/>
-        <color theme="10"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </ndxf>
-  </rcc>
-  <rcc rId="33" sId="5" odxf="1" dxf="1" numFmtId="19">
-    <nc r="E16">
-      <v>41711</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="34" sId="5">
-    <nc r="F16" t="inlineStr">
-      <is>
-        <t>Jan</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog9.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="35" sId="2" odxf="1" dxf="1">
-    <nc r="A9" t="inlineStr">
-      <is>
-        <t>Kpix</t>
-      </is>
-    </nc>
-    <odxf>
-      <alignment horizontal="center" vertical="top" readingOrder="0"/>
-    </odxf>
-    <ndxf>
-      <alignment horizontal="general" vertical="bottom" readingOrder="0"/>
-    </ndxf>
-  </rcc>
-  <rfmt sheetId="2" sqref="B9" start="0" length="0">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="C9" start="0" length="0">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="D9" start="0" length="0">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" s="1" sqref="E9" start="0" length="0">
-    <dxf>
-      <font>
-        <u/>
-        <sz val="12"/>
-        <color theme="10"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="F9" start="0" length="0">
-    <dxf>
-      <numFmt numFmtId="21" formatCode="dd\-mmm"/>
-      <alignment horizontal="general" vertical="bottom" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="G9" start="0" length="0">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="H9" start="0" length="0">
-    <dxf>
-      <numFmt numFmtId="21" formatCode="dd\-mmm"/>
-      <alignment horizontal="general" vertical="bottom" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="36" sId="2" odxf="1" dxf="1">
-    <nc r="I9" t="inlineStr">
-      <is>
-        <t>KPiX_RD_Status.docx</t>
-      </is>
-    </nc>
-    <odxf>
-      <alignment horizontal="center" vertical="top" readingOrder="0"/>
-    </odxf>
-    <ndxf>
-      <alignment horizontal="general" vertical="bottom" readingOrder="0"/>
-    </ndxf>
-  </rcc>
-  <rfmt sheetId="2" sqref="J9" start="0" length="0">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="37" sId="2">
-    <nc r="B9" t="inlineStr">
-      <is>
-        <t>SLAC</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="B9">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="38" sId="2">
-    <nc r="C9" t="inlineStr">
-      <is>
-        <t>Marty Breidenbach</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="39" sId="2">
-    <nc r="D9" t="inlineStr">
-      <is>
-        <t>mib@slac.stanford.edu</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="40" sId="2" odxf="1" dxf="1" numFmtId="19">
-    <nc r="E9">
-      <v>41711</v>
-    </nc>
-    <ndxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="41" sId="2">
-    <nc r="F9" t="inlineStr">
-      <is>
-        <t>Jan</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="42" sId="2" odxf="1" dxf="1" numFmtId="19">
-    <nc r="G9">
-      <v>41716</v>
-    </nc>
-    <ndxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="43" sId="2">
-    <nc r="H9" t="inlineStr">
-      <is>
-        <t>Report received</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcv guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" action="delete"/>
-  <rcv guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" action="add"/>
-</revisions>
-</file>
-
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
-  <userInfo guid="{5A5B8656-D36E-DD4B-A30D-CD5013FAD849}" name="Jan Strube" id="-985443287" dateTime="2014-04-23T12:14:53"/>
-</users>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3538,8 +1611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3562,10 +1635,10 @@
       <c r="B1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="37"/>
+      <c r="D1" s="39"/>
       <c r="E1" s="13" t="s">
         <v>1</v>
       </c>
@@ -3580,7 +1653,7 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="37" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3"/>
@@ -3595,7 +1668,7 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="39"/>
+      <c r="A3" s="37"/>
       <c r="B3" s="3"/>
       <c r="C3" s="38"/>
       <c r="D3" s="2" t="s">
@@ -3604,9 +1677,15 @@
       <c r="E3" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="F3" s="31">
+        <v>41754</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="39"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="3"/>
       <c r="C4" s="6" t="s">
         <v>7</v>
@@ -3625,10 +1704,10 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="37" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -3642,8 +1721,8 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="39"/>
-      <c r="B6" s="39"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="37"/>
       <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
@@ -3652,8 +1731,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="30">
-      <c r="A7" s="39"/>
-      <c r="B7" s="39"/>
+      <c r="A7" s="37"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="7" t="s">
         <v>20</v>
       </c>
@@ -3665,7 +1744,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="30">
-      <c r="A8" s="39"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
@@ -3680,7 +1759,7 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="37" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -3694,7 +1773,7 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="39"/>
+      <c r="A10" s="37"/>
       <c r="C10" s="38" t="s">
         <v>30</v>
       </c>
@@ -3706,7 +1785,7 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="39"/>
+      <c r="A11" s="37"/>
       <c r="C11" s="38"/>
       <c r="D11" t="s">
         <v>35</v>
@@ -3716,7 +1795,7 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="39"/>
+      <c r="A12" s="37"/>
       <c r="C12" s="6" t="s">
         <v>37</v>
       </c>
@@ -3728,7 +1807,7 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="37" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -3742,7 +1821,7 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="39"/>
+      <c r="A14" s="37"/>
       <c r="C14" s="6" t="s">
         <v>41</v>
       </c>
@@ -3754,7 +1833,7 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="39"/>
+      <c r="A15" s="37"/>
       <c r="C15" s="6" t="s">
         <v>29</v>
       </c>
@@ -3766,7 +1845,7 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="37" t="s">
         <v>44</v>
       </c>
       <c r="C16" t="s">
@@ -3780,7 +1859,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="30">
-      <c r="A17" s="39"/>
+      <c r="A17" s="37"/>
       <c r="C17" s="4" t="s">
         <v>48</v>
       </c>
@@ -3800,7 +1879,7 @@
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="37" t="s">
         <v>51</v>
       </c>
       <c r="C19" t="s">
@@ -3814,7 +1893,7 @@
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="39"/>
+      <c r="A20" s="37"/>
       <c r="C20" t="s">
         <v>45</v>
       </c>
@@ -3826,7 +1905,7 @@
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="37" t="s">
         <v>58</v>
       </c>
       <c r="C21" t="s">
@@ -3840,7 +1919,7 @@
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="39"/>
+      <c r="A22" s="37"/>
       <c r="B22" t="s">
         <v>65</v>
       </c>
@@ -3881,27 +1960,27 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" topLeftCell="B1">
+      <selection activeCell="H22" sqref="H22"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
       <selection activeCell="E24" sqref="E24"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" topLeftCell="B1">
-      <selection activeCell="H22" sqref="H22"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
   </customSheetViews>
   <mergeCells count="11">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A5:A8"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A19:A20"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A5:A8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
@@ -3960,10 +2039,10 @@
       <c r="A1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="37"/>
+      <c r="C1" s="39"/>
       <c r="D1" s="13" t="s">
         <v>1</v>
       </c>
@@ -3973,10 +2052,10 @@
       <c r="F1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="37"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="34" t="s">
@@ -4274,12 +2353,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
+      <selection activeCell="H16" sqref="H16"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" topLeftCell="B1">
       <selection activeCell="F14" sqref="F14"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
-      <selection activeCell="H16" sqref="H16"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
@@ -4327,10 +2406,10 @@
       <c r="A1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="37"/>
+      <c r="C1" s="39"/>
       <c r="D1" s="13" t="s">
         <v>1</v>
       </c>
@@ -4340,10 +2419,10 @@
       <c r="F1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="37"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="41" t="s">
@@ -4388,11 +2467,11 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
+      <selection activeCell="G5" sqref="G5"/>
+    </customSheetView>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
       <selection activeCell="E3" sqref="E3"/>
-    </customSheetView>
-    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
-      <selection activeCell="G5" sqref="G5"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="7">
@@ -4421,7 +2500,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4674,12 +2753,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
       <selection activeCell="C7" sqref="C7"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
@@ -4715,10 +2794,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4829,6 +2908,12 @@
       <c r="F5" t="s">
         <v>78</v>
       </c>
+      <c r="G5" s="15">
+        <v>41761</v>
+      </c>
+      <c r="H5" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="44"/>
@@ -4862,6 +2947,9 @@
       <c r="G7" s="15">
         <v>41723</v>
       </c>
+      <c r="H7" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="20" t="s">
@@ -5080,53 +3168,63 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="20"/>
+      <c r="E20" s="32"/>
+      <c r="G20" s="15">
+        <v>41765</v>
+      </c>
+      <c r="H20" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="20" t="s">
         <v>191</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>62</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>192</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
-      <c r="A24" t="s">
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
         <v>208</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>150</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>151</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>152</v>
       </c>
-      <c r="E24" s="26">
+      <c r="E25" s="26">
         <v>41711</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F25" t="s">
         <v>78</v>
       </c>
-      <c r="G24" s="26">
+      <c r="G25" s="26">
         <v>41716</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H25" t="s">
         <v>207</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
-      <selection activeCell="F8" sqref="F8"/>
-    </customSheetView>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
       <selection activeCell="G20" sqref="G20"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
+      <selection activeCell="F8" sqref="F8"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="5">
@@ -5146,7 +3244,7 @@
     <hyperlink ref="D11" r:id="rId7"/>
     <hyperlink ref="D12" r:id="rId8"/>
     <hyperlink ref="D14" r:id="rId9"/>
-    <hyperlink ref="D20" r:id="rId10"/>
+    <hyperlink ref="D21" r:id="rId10"/>
     <hyperlink ref="D16" r:id="rId11"/>
     <hyperlink ref="D5" r:id="rId12"/>
     <hyperlink ref="D3" r:id="rId13"/>
@@ -5171,8 +3269,8 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
   <customSheetViews>
+    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}"/>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}"/>
-    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}"/>
   </customSheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
adding contributions from dual readout
git-svn-id: svn+ssh://svn.cern.ch/reps/jansvn/trunk/lcDetRnD@553 4525493e-7705-40b1-a816-d608a930855b
</commit_message>
<xml_diff>
--- a/ListOfGroups.xlsx
+++ b/ListOfGroups.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="0" windowWidth="28720" windowHeight="17380" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="28720" windowHeight="17380" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TPC" sheetId="1" r:id="rId1"/>
     <sheet name="Vertex Detector" sheetId="2" r:id="rId2"/>
     <sheet name="Forward Calorimetry R&amp;D" sheetId="3" r:id="rId3"/>
     <sheet name="US Groups" sheetId="4" r:id="rId4"/>
-    <sheet name="Calice" sheetId="5" r:id="rId5"/>
+    <sheet name="Calorimetry" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet2" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="TITOV Maksym - Personal View" guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1243" windowHeight="652" tabRatio="500" activeSheetId="2"/>
     <customWorkbookView name="Jan Strube - Personal View" guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" mergeInterval="0" personalView="1" xWindow="-2" yWindow="54" windowWidth="1436" windowHeight="815" tabRatio="500" activeSheetId="5"/>
-    <customWorkbookView name="TITOV Maksym - Personal View" guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1243" windowHeight="652" tabRatio="500" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="251">
   <si>
     <t>Leader</t>
   </si>
@@ -805,6 +805,21 @@
   </si>
   <si>
     <t>Calorimeter_CLICdp_FrankSimon_MPI_20140506.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DualReadout </t>
+  </si>
+  <si>
+    <t>Iowa State</t>
+  </si>
+  <si>
+    <t>John Hauptman</t>
+  </si>
+  <si>
+    <t>hauptman@fnal.gov</t>
+  </si>
+  <si>
+    <t>DualReadout_JohnHauptman_IowaState_20140509.pdf</t>
   </si>
 </sst>
 </file>
@@ -990,14 +1005,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1037,7 +1052,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{AC3FBE52-88DD-8E4A-B5FB-5664F571FB55}" diskRevisions="1" revisionId="154" version="13">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{FCA1CE6A-80A0-7A48-81E6-BD057655BF9E}" diskRevisions="1" revisionId="163" version="14">
   <header guid="{71122420-D25E-0840-8EB5-EDCD8CABF1E4}" dateTime="2014-04-10T10:06:10" maxSheetId="8" userName="Jan Strube" r:id="rId28" minRId="135" maxRId="136">
     <sheetIdMap count="7">
       <sheetId val="1"/>
@@ -1083,6 +1098,17 @@
     </sheetIdMap>
   </header>
   <header guid="{AC3FBE52-88DD-8E4A-B5FB-5664F571FB55}" dateTime="2014-05-08T14:03:30" maxSheetId="8" userName="Jan Strube" r:id="rId32" minRId="147" maxRId="154">
+    <sheetIdMap count="7">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{FCA1CE6A-80A0-7A48-81E6-BD057655BF9E}" dateTime="2014-05-09T09:30:19" maxSheetId="8" userName="Jan Strube" r:id="rId33" minRId="155" maxRId="163">
     <sheetIdMap count="7">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1155,6 +1181,76 @@
       </is>
     </nc>
   </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="155" sId="5">
+    <nc r="A27" t="inlineStr">
+      <is>
+        <t xml:space="preserve">DualReadout </t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="156" sId="5">
+    <nc r="B27" t="inlineStr">
+      <is>
+        <t>Iowa State</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="157" sId="5">
+    <nc r="C27" t="inlineStr">
+      <is>
+        <t>John Hauptman</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="158" sId="5" xfDxf="1" dxf="1">
+    <nc r="D27" t="inlineStr">
+      <is>
+        <t>hauptman@fnal.gov</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="159" sId="5" odxf="1" dxf="1" numFmtId="21">
+    <nc r="E27">
+      <v>41757</v>
+    </nc>
+    <odxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </odxf>
+    <ndxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="160" sId="5">
+    <nc r="F27" t="inlineStr">
+      <is>
+        <t>Jan</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="161" sId="5" odxf="1" dxf="1" numFmtId="21">
+    <nc r="G27">
+      <v>41768</v>
+    </nc>
+    <odxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </odxf>
+    <ndxf>
+      <numFmt numFmtId="21" formatCode="d\-mmm"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="162" sId="5" xfDxf="1" dxf="1">
+    <nc r="H27" t="inlineStr">
+      <is>
+        <t>DualReadout_JohnHauptman_IowaState_20140509.pdf</t>
+      </is>
+    </nc>
+  </rcc>
+  <rsnm rId="163" sheetId="5" oldName="[ListOfGroups.xlsx]Calice" newName="[ListOfGroups.xlsx]Calorimetry"/>
 </revisions>
 </file>
 
@@ -1611,8 +1707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1635,10 +1731,10 @@
       <c r="B1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="39"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="13" t="s">
         <v>1</v>
       </c>
@@ -1653,7 +1749,7 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3"/>
@@ -1668,7 +1764,7 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="37"/>
+      <c r="A3" s="39"/>
       <c r="B3" s="3"/>
       <c r="C3" s="38"/>
       <c r="D3" s="2" t="s">
@@ -1685,7 +1781,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="37"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="3"/>
       <c r="C4" s="6" t="s">
         <v>7</v>
@@ -1704,10 +1800,10 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="39" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -1721,8 +1817,8 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="37"/>
-      <c r="B6" s="37"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="39"/>
       <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
@@ -1731,8 +1827,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="30">
-      <c r="A7" s="37"/>
-      <c r="B7" s="37"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="39"/>
       <c r="C7" s="7" t="s">
         <v>20</v>
       </c>
@@ -1744,7 +1840,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="30">
-      <c r="A8" s="37"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
@@ -1759,7 +1855,7 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="39" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -1773,7 +1869,7 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="37"/>
+      <c r="A10" s="39"/>
       <c r="C10" s="38" t="s">
         <v>30</v>
       </c>
@@ -1785,7 +1881,7 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="37"/>
+      <c r="A11" s="39"/>
       <c r="C11" s="38"/>
       <c r="D11" t="s">
         <v>35</v>
@@ -1795,7 +1891,7 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="37"/>
+      <c r="A12" s="39"/>
       <c r="C12" s="6" t="s">
         <v>37</v>
       </c>
@@ -1807,7 +1903,7 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="39" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -1821,7 +1917,7 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="37"/>
+      <c r="A14" s="39"/>
       <c r="C14" s="6" t="s">
         <v>41</v>
       </c>
@@ -1833,7 +1929,7 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="37"/>
+      <c r="A15" s="39"/>
       <c r="C15" s="6" t="s">
         <v>29</v>
       </c>
@@ -1845,7 +1941,7 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="39" t="s">
         <v>44</v>
       </c>
       <c r="C16" t="s">
@@ -1859,7 +1955,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="30">
-      <c r="A17" s="37"/>
+      <c r="A17" s="39"/>
       <c r="C17" s="4" t="s">
         <v>48</v>
       </c>
@@ -1879,7 +1975,7 @@
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="39" t="s">
         <v>51</v>
       </c>
       <c r="C19" t="s">
@@ -1893,7 +1989,7 @@
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="37"/>
+      <c r="A20" s="39"/>
       <c r="C20" t="s">
         <v>45</v>
       </c>
@@ -1905,7 +2001,7 @@
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="39" t="s">
         <v>58</v>
       </c>
       <c r="C21" t="s">
@@ -1919,7 +2015,7 @@
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="37"/>
+      <c r="A22" s="39"/>
       <c r="B22" t="s">
         <v>65</v>
       </c>
@@ -1960,27 +2056,27 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
+      <selection activeCell="E24" sqref="E24"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" topLeftCell="B1">
       <selection activeCell="H22" sqref="H22"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
-      <selection activeCell="E24" sqref="E24"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
   </customSheetViews>
   <mergeCells count="11">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A5:A8"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A19:A20"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A5:A8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
@@ -2039,10 +2135,10 @@
       <c r="A1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="39"/>
+      <c r="C1" s="37"/>
       <c r="D1" s="13" t="s">
         <v>1</v>
       </c>
@@ -2052,10 +2148,10 @@
       <c r="F1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="39"/>
+      <c r="H1" s="37"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="34" t="s">
@@ -2353,12 +2449,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" topLeftCell="B1">
+      <selection activeCell="F14" sqref="F14"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
       <selection activeCell="H16" sqref="H16"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" topLeftCell="B1">
-      <selection activeCell="F14" sqref="F14"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
@@ -2406,10 +2502,10 @@
       <c r="A1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="39"/>
+      <c r="C1" s="37"/>
       <c r="D1" s="13" t="s">
         <v>1</v>
       </c>
@@ -2419,10 +2515,10 @@
       <c r="F1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="39"/>
+      <c r="H1" s="37"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="41" t="s">
@@ -2467,11 +2563,11 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
+      <selection activeCell="E3" sqref="E3"/>
+    </customSheetView>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
       <selection activeCell="G5" sqref="G5"/>
-    </customSheetView>
-    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
-      <selection activeCell="E3" sqref="E3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="7">
@@ -2500,7 +2596,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2753,12 +2849,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
+      <selection activeCell="C7" sqref="C7"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
       <selection activeCell="A6" sqref="A6:XFD6"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
-      <selection activeCell="C7" sqref="C7"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
@@ -2794,10 +2890,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3217,14 +3313,40 @@
         <v>207</v>
       </c>
     </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>246</v>
+      </c>
+      <c r="B27" t="s">
+        <v>247</v>
+      </c>
+      <c r="C27" t="s">
+        <v>248</v>
+      </c>
+      <c r="D27" t="s">
+        <v>249</v>
+      </c>
+      <c r="E27" s="15">
+        <v>41757</v>
+      </c>
+      <c r="F27" t="s">
+        <v>78</v>
+      </c>
+      <c r="G27" s="15">
+        <v>41768</v>
+      </c>
+      <c r="H27" t="s">
+        <v>250</v>
+      </c>
+    </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
+      <selection activeCell="F8" sqref="F8"/>
+    </customSheetView>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
       <selection activeCell="G20" sqref="G20"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
-      <selection activeCell="F8" sqref="F8"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="5">
@@ -3269,8 +3391,8 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
   <customSheetViews>
+    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}"/>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}"/>
-    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}"/>
   </customSheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Adding contribution from Annecy
git-svn-id: svn+ssh://svn.cern.ch/reps/jansvn/trunk/lcDetRnD@555 4525493e-7705-40b1-a816-d608a930855b
</commit_message>
<xml_diff>
--- a/ListOfGroups.xlsx
+++ b/ListOfGroups.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="28720" windowHeight="17380" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="-40" yWindow="0" windowWidth="28720" windowHeight="17380" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TPC" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,8 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jan Strube - Personal View" guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" mergeInterval="0" personalView="1" xWindow="-2" yWindow="54" windowWidth="1436" windowHeight="815" tabRatio="500" activeSheetId="5"/>
     <customWorkbookView name="TITOV Maksym - Personal View" guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1243" windowHeight="652" tabRatio="500" activeSheetId="2"/>
-    <customWorkbookView name="Jan Strube - Personal View" guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" mergeInterval="0" personalView="1" xWindow="-2" yWindow="54" windowWidth="1436" windowHeight="815" tabRatio="500" activeSheetId="5"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="252">
   <si>
     <t>Leader</t>
   </si>
@@ -820,6 +820,9 @@
   </si>
   <si>
     <t>DualReadout_JohnHauptman_IowaState_20140509.pdf</t>
+  </si>
+  <si>
+    <t>SDHCal_MaximilienChefdeville_Annecy_20140516.pdf</t>
   </si>
 </sst>
 </file>
@@ -1005,14 +1008,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1052,40 +1055,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{FCA1CE6A-80A0-7A48-81E6-BD057655BF9E}" diskRevisions="1" revisionId="163" version="14">
-  <header guid="{71122420-D25E-0840-8EB5-EDCD8CABF1E4}" dateTime="2014-04-10T10:06:10" maxSheetId="8" userName="Jan Strube" r:id="rId28" minRId="135" maxRId="136">
-    <sheetIdMap count="7">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-      <sheetId val="6"/>
-      <sheetId val="7"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{6BCB8514-64F9-584F-929A-31E5D59EA1D8}" dateTime="2014-04-10T22:52:05" maxSheetId="8" userName="Jan Strube" r:id="rId29" minRId="137" maxRId="138">
-    <sheetIdMap count="7">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-      <sheetId val="6"/>
-      <sheetId val="7"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{0E50AB3B-3EA7-0C4A-B94E-AD02E868D3B2}" dateTime="2014-04-15T16:45:48" maxSheetId="8" userName="Jan Strube" r:id="rId30" minRId="139" maxRId="140">
-    <sheetIdMap count="7">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-      <sheetId val="6"/>
-      <sheetId val="7"/>
-    </sheetIdMap>
-  </header>
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{58887AFD-FB25-684E-B4EF-A3D84F19E69B}" diskRevisions="1" revisionId="165" version="15">
   <header guid="{5A5B8656-D36E-DD4B-A30D-CD5013FAD849}" dateTime="2014-04-23T12:19:34" maxSheetId="8" userName="Jan Strube" r:id="rId31" minRId="141" maxRId="146">
     <sheetIdMap count="7">
       <sheetId val="1"/>
@@ -1109,6 +1079,17 @@
     </sheetIdMap>
   </header>
   <header guid="{FCA1CE6A-80A0-7A48-81E6-BD057655BF9E}" dateTime="2014-05-09T09:30:19" maxSheetId="8" userName="Jan Strube" r:id="rId33" minRId="155" maxRId="163">
+    <sheetIdMap count="7">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{58887AFD-FB25-684E-B4EF-A3D84F19E69B}" dateTime="2014-05-17T11:55:58" maxSheetId="8" userName="Jan Strube" r:id="rId34" minRId="164" maxRId="165">
     <sheetIdMap count="7">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1254,11 +1235,11 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="135" sId="5" odxf="1" dxf="1" numFmtId="21">
-    <nc r="G9">
-      <v>41739</v>
+  <rcc rId="164" sId="5" odxf="1" dxf="1" numFmtId="21">
+    <nc r="G14">
+      <v>41775</v>
     </nc>
     <odxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1267,53 +1248,10 @@
       <numFmt numFmtId="21" formatCode="d\-mmm"/>
     </ndxf>
   </rcc>
-  <rcc rId="136" sId="5">
-    <nc r="H9" t="inlineStr">
+  <rcc rId="165" sId="5" xfDxf="1" dxf="1">
+    <nc r="H14" t="inlineStr">
       <is>
-        <t>AHCAL_FelixSefkow_DESY_20140410.docx</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog29.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="137" sId="2" numFmtId="19">
-    <nc r="G6">
-      <v>41739</v>
-    </nc>
-  </rcc>
-  <rcc rId="138" sId="2" xfDxf="1" dxf="1">
-    <nc r="H6" t="inlineStr">
-      <is>
-        <t>3DPixel_RonLipton_FNAL_20140410.docx</t>
-      </is>
-    </nc>
-    <ndxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </ndxf>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog30.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="139" sId="5" odxf="1" dxf="1" numFmtId="21">
-    <nc r="G10">
-      <v>41740</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="140" sId="5">
-    <nc r="H10" t="inlineStr">
-      <is>
-        <t>DHCAL_JoseRepond_ANL_20140411.docx</t>
+        <t>SDHCal_MaximilienChefdeville_Annecy_20140516.pdf</t>
       </is>
     </nc>
   </rcc>
@@ -1731,10 +1669,10 @@
       <c r="B1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="37"/>
+      <c r="D1" s="39"/>
       <c r="E1" s="13" t="s">
         <v>1</v>
       </c>
@@ -1749,7 +1687,7 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="37" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3"/>
@@ -1764,7 +1702,7 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="39"/>
+      <c r="A3" s="37"/>
       <c r="B3" s="3"/>
       <c r="C3" s="38"/>
       <c r="D3" s="2" t="s">
@@ -1781,7 +1719,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="39"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="3"/>
       <c r="C4" s="6" t="s">
         <v>7</v>
@@ -1800,10 +1738,10 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="37" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -1817,8 +1755,8 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="39"/>
-      <c r="B6" s="39"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="37"/>
       <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
@@ -1827,8 +1765,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="30">
-      <c r="A7" s="39"/>
-      <c r="B7" s="39"/>
+      <c r="A7" s="37"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="7" t="s">
         <v>20</v>
       </c>
@@ -1840,7 +1778,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="30">
-      <c r="A8" s="39"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
@@ -1855,7 +1793,7 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="37" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -1869,7 +1807,7 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="39"/>
+      <c r="A10" s="37"/>
       <c r="C10" s="38" t="s">
         <v>30</v>
       </c>
@@ -1881,7 +1819,7 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="39"/>
+      <c r="A11" s="37"/>
       <c r="C11" s="38"/>
       <c r="D11" t="s">
         <v>35</v>
@@ -1891,7 +1829,7 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="39"/>
+      <c r="A12" s="37"/>
       <c r="C12" s="6" t="s">
         <v>37</v>
       </c>
@@ -1903,7 +1841,7 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="37" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -1917,7 +1855,7 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="39"/>
+      <c r="A14" s="37"/>
       <c r="C14" s="6" t="s">
         <v>41</v>
       </c>
@@ -1929,7 +1867,7 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="39"/>
+      <c r="A15" s="37"/>
       <c r="C15" s="6" t="s">
         <v>29</v>
       </c>
@@ -1941,7 +1879,7 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="37" t="s">
         <v>44</v>
       </c>
       <c r="C16" t="s">
@@ -1955,7 +1893,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="30">
-      <c r="A17" s="39"/>
+      <c r="A17" s="37"/>
       <c r="C17" s="4" t="s">
         <v>48</v>
       </c>
@@ -1975,7 +1913,7 @@
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="37" t="s">
         <v>51</v>
       </c>
       <c r="C19" t="s">
@@ -1989,7 +1927,7 @@
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="39"/>
+      <c r="A20" s="37"/>
       <c r="C20" t="s">
         <v>45</v>
       </c>
@@ -2001,7 +1939,7 @@
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="37" t="s">
         <v>58</v>
       </c>
       <c r="C21" t="s">
@@ -2015,7 +1953,7 @@
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="39"/>
+      <c r="A22" s="37"/>
       <c r="B22" t="s">
         <v>65</v>
       </c>
@@ -2056,27 +1994,27 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" topLeftCell="B1">
+      <selection activeCell="H22" sqref="H22"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
       <selection activeCell="E24" sqref="E24"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}" topLeftCell="B1">
-      <selection activeCell="H22" sqref="H22"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
   </customSheetViews>
   <mergeCells count="11">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A5:A8"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A19:A20"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A5:A8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
@@ -2135,10 +2073,10 @@
       <c r="A1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="37"/>
+      <c r="C1" s="39"/>
       <c r="D1" s="13" t="s">
         <v>1</v>
       </c>
@@ -2148,10 +2086,10 @@
       <c r="F1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="37"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="34" t="s">
@@ -2449,12 +2387,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
+      <selection activeCell="H16" sqref="H16"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}" topLeftCell="B1">
       <selection activeCell="F14" sqref="F14"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
-      <selection activeCell="H16" sqref="H16"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
@@ -2502,10 +2440,10 @@
       <c r="A1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="37"/>
+      <c r="C1" s="39"/>
       <c r="D1" s="13" t="s">
         <v>1</v>
       </c>
@@ -2515,10 +2453,10 @@
       <c r="F1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="37"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="41" t="s">
@@ -2563,11 +2501,11 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
+      <selection activeCell="G5" sqref="G5"/>
+    </customSheetView>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
       <selection activeCell="E3" sqref="E3"/>
-    </customSheetView>
-    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
-      <selection activeCell="G5" sqref="G5"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="7">
@@ -2849,12 +2787,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
       <selection activeCell="C7" sqref="C7"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>
@@ -2893,7 +2831,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3197,6 +3135,12 @@
       <c r="F14" t="s">
         <v>72</v>
       </c>
+      <c r="G14" s="15">
+        <v>41775</v>
+      </c>
+      <c r="H14" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="20" t="s">
@@ -3341,12 +3285,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
-      <selection activeCell="F8" sqref="F8"/>
-    </customSheetView>
     <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}">
       <selection activeCell="G20" sqref="G20"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}">
+      <selection activeCell="F8" sqref="F8"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="5">
@@ -3391,8 +3335,8 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
   <customSheetViews>
+    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}"/>
     <customSheetView guid="{24320570-5786-4ED4-AD1D-A7698491F5AB}"/>
-    <customSheetView guid="{7FE15BB2-DE7C-DC45-9455-01C8CFCD0F6D}"/>
   </customSheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Adding references to the bibliography. Adding support for caliceanalysisnotes in the bibliography
git-svn-id: svn+ssh://svn.cern.ch/reps/jansvn/trunk/lcDetRnD@558 4525493e-7705-40b1-a816-d608a930855b
</commit_message>
<xml_diff>
--- a/ListOfGroups.xlsx
+++ b/ListOfGroups.xlsx
@@ -1056,17 +1056,6 @@
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
 <headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{58887AFD-FB25-684E-B4EF-A3D84F19E69B}" diskRevisions="1" revisionId="165" version="15">
-  <header guid="{5A5B8656-D36E-DD4B-A30D-CD5013FAD849}" dateTime="2014-04-23T12:19:34" maxSheetId="8" userName="Jan Strube" r:id="rId31" minRId="141" maxRId="146">
-    <sheetIdMap count="7">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-      <sheetId val="5"/>
-      <sheetId val="6"/>
-      <sheetId val="7"/>
-    </sheetIdMap>
-  </header>
   <header guid="{AC3FBE52-88DD-8E4A-B5FB-5664F571FB55}" dateTime="2014-05-08T14:03:30" maxSheetId="8" userName="Jan Strube" r:id="rId32" minRId="147" maxRId="154">
     <sheetIdMap count="7">
       <sheetId val="1"/>
@@ -1254,65 +1243,6 @@
         <t>SDHCal_MaximilienChefdeville_Annecy_20140516.pdf</t>
       </is>
     </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog31.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="141" sId="5" odxf="1" dxf="1" numFmtId="21">
-    <nc r="G11">
-      <v>41751</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
-    </ndxf>
-  </rcc>
-  <rfmt sheetId="5" xfDxf="1" sqref="H11" start="0" length="0"/>
-  <rcc rId="142" sId="5" xfDxf="1" dxf="1">
-    <nc r="H11" t="inlineStr">
-      <is>
-        <t>SDHCal_ImadLaktineh_IN2P3_20140422.pdf</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="143" sId="5" odxf="1" dxf="1" numFmtId="21">
-    <nc r="G4">
-      <v>41750</v>
-    </nc>
-    <odxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </odxf>
-    <ndxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
-    </ndxf>
-  </rcc>
-  <rfmt sheetId="5" xfDxf="1" sqref="H4" start="0" length="0"/>
-  <rcc rId="144" sId="5">
-    <nc r="H4" t="inlineStr">
-      <is>
-        <t>Calorimeter_SiliconTungstenILD_RomanPoeschl_LAL_20140421.pdf</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="5" xfDxf="1" sqref="G3" start="0" length="0"/>
-  <rcc rId="145" sId="5" xfDxf="1" dxf="1">
-    <nc r="H3" t="inlineStr">
-      <is>
-        <t>Calorimeter_SiliconTungstenILD_VincentBoudry_IN2P3_20140323.docx</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="146" sId="5" odxf="1" dxf="1" numFmtId="21">
-    <nc r="G3">
-      <v>41721</v>
-    </nc>
-    <ndxf>
-      <numFmt numFmtId="21" formatCode="d\-mmm"/>
-    </ndxf>
   </rcc>
 </revisions>
 </file>

</xml_diff>